<commit_message>
subjects and samples improve field descriptions
</commit_message>
<xml_diff>
--- a/resources/DatasetTemplate/samples.xlsx
+++ b/resources/DatasetTemplate/samples.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t xml:space="preserve">subject_id</t>
   </si>
@@ -91,10 +91,16 @@
     <t xml:space="preserve">Lab-based schema for identifying each subject</t>
   </si>
   <si>
+    <t xml:space="preserve">Lab-based schema for identifying each sample, must be unique</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sample_id of the sample from which the current sample was derived (e.g., slice, tissue punch, biopsy, etc.)</t>
+  </si>
+  <si>
     <t xml:space="preserve">If data is collected on multiple samples at the same time include the identifier of the pool where the data file will be found.</t>
   </si>
   <si>
-    <t xml:space="preserve">Experimental group subject is assigned to in research project</t>
+    <t xml:space="preserve">Experimental group subject is assigned to in research project. If you have experimental groups for samples please add another column.</t>
   </si>
   <si>
     <t xml:space="preserve">Physical type of the specimen from which the data were extracted</t>
@@ -635,66 +641,66 @@
         <v>22</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H2" s="0"/>
       <c r="I2" s="8" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="K2" s="8" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="M2" s="8" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="O2" s="8" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="P2" s="9" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="Q2" s="12" t="str">
         <f aca="false">HYPERLINK("https://scicrunch.org/resources/Organisms/search","RRID for the strain For this field")</f>
         <v>RRID for the strain For this field</v>
       </c>
       <c r="R2" s="9" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="S2" s="9" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="T2" s="9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="U2" s="8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="V2" s="8" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="W2" s="0"/>
       <c r="X2" s="0"/>
@@ -705,65 +711,65 @@
     </row>
     <row r="3" s="7" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="9" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H3" s="0"/>
       <c r="I3" s="9" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="N3" s="9" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="O3" s="9" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="P3" s="9" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="Q3" s="9" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="R3" s="9" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="S3" s="9" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="T3" s="9" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="U3" s="13" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="V3" s="14"/>
       <c r="W3" s="0"/>

</xml_diff>

<commit_message>
dataset template fix typo in samples/subjects
and version bump the template to account for the change
</commit_message>
<xml_diff>
--- a/resources/DatasetTemplate/samples.xlsx
+++ b/resources/DatasetTemplate/samples.xlsx
@@ -61,7 +61,7 @@
     <t xml:space="preserve">age range (min)</t>
   </si>
   <si>
-    <t xml:space="preserve">age range (max) disease</t>
+    <t xml:space="preserve">age range (max)</t>
   </si>
   <si>
     <t xml:space="preserve">handedness</t>
@@ -530,8 +530,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
samples file reorder columsn for better workflow
also switched to align header text to center
</commit_message>
<xml_diff>
--- a/resources/DatasetTemplate/samples.xlsx
+++ b/resources/DatasetTemplate/samples.xlsx
@@ -34,12 +34,6 @@
     <t xml:space="preserve">pool id</t>
   </si>
   <si>
-    <t xml:space="preserve">member of</t>
-  </si>
-  <si>
-    <t xml:space="preserve">also in dataset</t>
-  </si>
-  <si>
     <t xml:space="preserve">sample experimental group</t>
   </si>
   <si>
@@ -47,6 +41,12 @@
   </si>
   <si>
     <t xml:space="preserve">sample anatomical location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">also in dataset</t>
+  </si>
+  <si>
+    <t xml:space="preserve">member of</t>
   </si>
   <si>
     <t xml:space="preserve">laboratory internal id</t>
@@ -222,23 +222,23 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -336,27 +336,27 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="19.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="30.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="14.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="29.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="23.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="20.08"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="28.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="17.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="11.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="10.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="10.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="14.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="20.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="14.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="22.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="22.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="15.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="21.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="13.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="9.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="8.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="8.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="13.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="11.51"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="15.79"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -372,19 +372,19 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="5" t="s">
@@ -422,9 +422,9 @@
       <c r="A2" s="7"/>
       <c r="B2" s="7"/>
       <c r="C2" s="7"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
       <c r="J2" s="7"/>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
@@ -434,9 +434,10 @@
       <c r="A3" s="9"/>
       <c r="B3" s="9"/>
       <c r="C3" s="7"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="I3" s="7"/>
       <c r="J3" s="9"/>
       <c r="K3" s="9"/>
       <c r="L3" s="9"/>
@@ -446,9 +447,10 @@
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
       <c r="C4" s="9"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
+      <c r="I4" s="7"/>
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
@@ -458,9 +460,9 @@
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
       <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
@@ -470,9 +472,9 @@
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
       <c r="G6" s="9"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
@@ -482,9 +484,9 @@
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
       <c r="G7" s="9"/>
-      <c r="H7" s="9"/>
-      <c r="I7" s="9"/>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
@@ -494,9 +496,9 @@
       <c r="A8" s="9"/>
       <c r="B8" s="9"/>
       <c r="C8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
       <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
@@ -506,9 +508,9 @@
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
       <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
       <c r="L9" s="9"/>
@@ -518,9 +520,9 @@
       <c r="A10" s="9"/>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
       <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
       <c r="L10" s="9"/>
@@ -530,9 +532,9 @@
       <c r="A11" s="9"/>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
       <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
       <c r="L11" s="9"/>
@@ -542,9 +544,9 @@
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
       <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
       <c r="L12" s="9"/>
@@ -554,9 +556,9 @@
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
       <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
@@ -566,9 +568,9 @@
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="9"/>
       <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
-      <c r="I14" s="9"/>
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
       <c r="L14" s="9"/>
@@ -578,9 +580,9 @@
       <c r="A15" s="9"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
       <c r="G15" s="9"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="9"/>
       <c r="J15" s="9"/>
       <c r="K15" s="9"/>
       <c r="L15" s="9"/>
@@ -590,9 +592,9 @@
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
       <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
       <c r="L16" s="9"/>
@@ -602,9 +604,9 @@
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
       <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
       <c r="L17" s="9"/>
@@ -614,9 +616,9 @@
       <c r="A18" s="9"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
       <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9"/>
       <c r="J18" s="9"/>
       <c r="K18" s="9"/>
       <c r="L18" s="9"/>
@@ -626,9 +628,9 @@
       <c r="A19" s="9"/>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
       <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
       <c r="J19" s="9"/>
       <c r="K19" s="9"/>
       <c r="L19" s="9"/>
@@ -638,9 +640,9 @@
       <c r="A20" s="9"/>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
       <c r="G20" s="9"/>
-      <c r="H20" s="9"/>
-      <c r="I20" s="9"/>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
       <c r="L20" s="9"/>
@@ -650,9 +652,9 @@
       <c r="A21" s="9"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
       <c r="G21" s="9"/>
-      <c r="H21" s="9"/>
-      <c r="I21" s="9"/>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
       <c r="L21" s="9"/>
@@ -662,9 +664,9 @@
       <c r="A22" s="9"/>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
       <c r="G22" s="9"/>
-      <c r="H22" s="9"/>
-      <c r="I22" s="9"/>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
       <c r="L22" s="9"/>
@@ -674,9 +676,9 @@
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
       <c r="G23" s="9"/>
-      <c r="H23" s="9"/>
-      <c r="I23" s="9"/>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
       <c r="L23" s="9"/>
@@ -686,9 +688,9 @@
       <c r="A24" s="9"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
       <c r="G24" s="9"/>
-      <c r="H24" s="9"/>
-      <c r="I24" s="9"/>
       <c r="J24" s="9"/>
       <c r="K24" s="9"/>
       <c r="L24" s="9"/>
@@ -698,9 +700,9 @@
       <c r="A25" s="9"/>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
       <c r="G25" s="9"/>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9"/>
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
       <c r="L25" s="9"/>
@@ -710,9 +712,9 @@
       <c r="A26" s="9"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
       <c r="G26" s="9"/>
-      <c r="H26" s="9"/>
-      <c r="I26" s="9"/>
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
       <c r="L26" s="9"/>
@@ -722,9 +724,9 @@
       <c r="A27" s="9"/>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
       <c r="G27" s="9"/>
-      <c r="H27" s="9"/>
-      <c r="I27" s="9"/>
       <c r="J27" s="9"/>
       <c r="K27" s="9"/>
       <c r="L27" s="9"/>
@@ -734,9 +736,9 @@
       <c r="A28" s="9"/>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
       <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
       <c r="J28" s="9"/>
       <c r="K28" s="9"/>
       <c r="L28" s="9"/>
@@ -746,9 +748,9 @@
       <c r="A29" s="9"/>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
       <c r="G29" s="9"/>
-      <c r="H29" s="9"/>
-      <c r="I29" s="9"/>
       <c r="J29" s="9"/>
       <c r="K29" s="9"/>
       <c r="L29" s="9"/>
@@ -758,9 +760,9 @@
       <c r="A30" s="9"/>
       <c r="B30" s="9"/>
       <c r="C30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
       <c r="G30" s="9"/>
-      <c r="H30" s="9"/>
-      <c r="I30" s="9"/>
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
       <c r="L30" s="9"/>
@@ -770,9 +772,9 @@
       <c r="A31" s="9"/>
       <c r="B31" s="9"/>
       <c r="C31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
       <c r="G31" s="9"/>
-      <c r="H31" s="9"/>
-      <c r="I31" s="9"/>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
       <c r="L31" s="9"/>
@@ -782,9 +784,9 @@
       <c r="A32" s="9"/>
       <c r="B32" s="9"/>
       <c r="C32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
       <c r="G32" s="9"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="9"/>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
       <c r="L32" s="9"/>
@@ -794,9 +796,9 @@
       <c r="A33" s="9"/>
       <c r="B33" s="9"/>
       <c r="C33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
       <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="I33" s="9"/>
       <c r="J33" s="9"/>
       <c r="K33" s="9"/>
       <c r="L33" s="9"/>
@@ -806,9 +808,9 @@
       <c r="A34" s="9"/>
       <c r="B34" s="9"/>
       <c r="C34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
       <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="9"/>
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
       <c r="L34" s="9"/>
@@ -818,9 +820,9 @@
       <c r="A35" s="9"/>
       <c r="B35" s="9"/>
       <c r="C35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
       <c r="G35" s="9"/>
-      <c r="H35" s="9"/>
-      <c r="I35" s="9"/>
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
       <c r="L35" s="9"/>
@@ -830,9 +832,9 @@
       <c r="A36" s="9"/>
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
       <c r="G36" s="9"/>
-      <c r="H36" s="9"/>
-      <c r="I36" s="9"/>
       <c r="J36" s="9"/>
       <c r="K36" s="9"/>
       <c r="L36" s="9"/>
@@ -842,9 +844,9 @@
       <c r="A37" s="9"/>
       <c r="B37" s="9"/>
       <c r="C37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
       <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="9"/>
       <c r="J37" s="9"/>
       <c r="K37" s="9"/>
       <c r="L37" s="9"/>
@@ -854,9 +856,9 @@
       <c r="A38" s="9"/>
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
       <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
-      <c r="I38" s="9"/>
       <c r="J38" s="9"/>
       <c r="K38" s="9"/>
       <c r="L38" s="9"/>
@@ -866,9 +868,9 @@
       <c r="A39" s="9"/>
       <c r="B39" s="9"/>
       <c r="C39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
       <c r="G39" s="9"/>
-      <c r="H39" s="9"/>
-      <c r="I39" s="9"/>
       <c r="J39" s="9"/>
       <c r="K39" s="9"/>
       <c r="L39" s="9"/>
@@ -878,9 +880,9 @@
       <c r="A40" s="9"/>
       <c r="B40" s="9"/>
       <c r="C40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
       <c r="G40" s="9"/>
-      <c r="H40" s="9"/>
-      <c r="I40" s="9"/>
       <c r="J40" s="9"/>
       <c r="K40" s="9"/>
       <c r="L40" s="9"/>
@@ -890,9 +892,9 @@
       <c r="A41" s="9"/>
       <c r="B41" s="9"/>
       <c r="C41" s="9"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
       <c r="G41" s="9"/>
-      <c r="H41" s="9"/>
-      <c r="I41" s="9"/>
       <c r="J41" s="9"/>
       <c r="K41" s="9"/>
       <c r="L41" s="9"/>
@@ -902,9 +904,9 @@
       <c r="A42" s="9"/>
       <c r="B42" s="9"/>
       <c r="C42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
       <c r="G42" s="9"/>
-      <c r="H42" s="9"/>
-      <c r="I42" s="9"/>
       <c r="J42" s="9"/>
       <c r="K42" s="9"/>
       <c r="L42" s="9"/>
@@ -914,9 +916,9 @@
       <c r="A43" s="9"/>
       <c r="B43" s="9"/>
       <c r="C43" s="9"/>
+      <c r="E43" s="9"/>
+      <c r="F43" s="9"/>
       <c r="G43" s="9"/>
-      <c r="H43" s="9"/>
-      <c r="I43" s="9"/>
       <c r="J43" s="9"/>
       <c r="K43" s="9"/>
       <c r="L43" s="9"/>
@@ -926,9 +928,9 @@
       <c r="A44" s="9"/>
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
+      <c r="E44" s="9"/>
+      <c r="F44" s="9"/>
       <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="9"/>
       <c r="J44" s="9"/>
       <c r="K44" s="9"/>
       <c r="L44" s="9"/>
@@ -938,9 +940,9 @@
       <c r="A45" s="9"/>
       <c r="B45" s="9"/>
       <c r="C45" s="9"/>
+      <c r="E45" s="9"/>
+      <c r="F45" s="9"/>
       <c r="G45" s="9"/>
-      <c r="H45" s="9"/>
-      <c r="I45" s="9"/>
       <c r="J45" s="9"/>
       <c r="K45" s="9"/>
       <c r="L45" s="9"/>
@@ -950,9 +952,9 @@
       <c r="A46" s="9"/>
       <c r="B46" s="9"/>
       <c r="C46" s="9"/>
+      <c r="E46" s="9"/>
+      <c r="F46" s="9"/>
       <c r="G46" s="9"/>
-      <c r="H46" s="9"/>
-      <c r="I46" s="9"/>
       <c r="J46" s="9"/>
       <c r="K46" s="9"/>
       <c r="L46" s="9"/>
@@ -962,9 +964,9 @@
       <c r="A47" s="9"/>
       <c r="B47" s="9"/>
       <c r="C47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="9"/>
       <c r="G47" s="9"/>
-      <c r="H47" s="9"/>
-      <c r="I47" s="9"/>
       <c r="J47" s="9"/>
       <c r="K47" s="9"/>
       <c r="L47" s="9"/>
@@ -974,9 +976,9 @@
       <c r="A48" s="9"/>
       <c r="B48" s="9"/>
       <c r="C48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="9"/>
       <c r="G48" s="9"/>
-      <c r="H48" s="9"/>
-      <c r="I48" s="9"/>
       <c r="J48" s="9"/>
       <c r="K48" s="9"/>
       <c r="L48" s="9"/>
@@ -986,9 +988,9 @@
       <c r="A49" s="9"/>
       <c r="B49" s="9"/>
       <c r="C49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="9"/>
       <c r="G49" s="9"/>
-      <c r="H49" s="9"/>
-      <c r="I49" s="9"/>
       <c r="J49" s="9"/>
       <c r="K49" s="9"/>
       <c r="L49" s="9"/>
@@ -998,9 +1000,9 @@
       <c r="A50" s="9"/>
       <c r="B50" s="9"/>
       <c r="C50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="9"/>
       <c r="G50" s="9"/>
-      <c r="H50" s="9"/>
-      <c r="I50" s="9"/>
       <c r="J50" s="9"/>
       <c r="K50" s="9"/>
       <c r="L50" s="9"/>
@@ -1010,9 +1012,9 @@
       <c r="A51" s="9"/>
       <c r="B51" s="9"/>
       <c r="C51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
       <c r="G51" s="9"/>
-      <c r="H51" s="9"/>
-      <c r="I51" s="9"/>
       <c r="J51" s="9"/>
       <c r="K51" s="9"/>
       <c r="L51" s="9"/>
@@ -1022,9 +1024,9 @@
       <c r="A52" s="9"/>
       <c r="B52" s="9"/>
       <c r="C52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="9"/>
       <c r="G52" s="9"/>
-      <c r="H52" s="9"/>
-      <c r="I52" s="9"/>
       <c r="J52" s="9"/>
       <c r="K52" s="9"/>
       <c r="L52" s="9"/>
@@ -1034,9 +1036,9 @@
       <c r="A53" s="9"/>
       <c r="B53" s="9"/>
       <c r="C53" s="9"/>
+      <c r="E53" s="9"/>
+      <c r="F53" s="9"/>
       <c r="G53" s="9"/>
-      <c r="H53" s="9"/>
-      <c r="I53" s="9"/>
       <c r="J53" s="9"/>
       <c r="K53" s="9"/>
       <c r="L53" s="9"/>
@@ -1046,9 +1048,9 @@
       <c r="A54" s="9"/>
       <c r="B54" s="9"/>
       <c r="C54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
       <c r="G54" s="9"/>
-      <c r="H54" s="9"/>
-      <c r="I54" s="9"/>
       <c r="J54" s="9"/>
       <c r="K54" s="9"/>
       <c r="L54" s="9"/>
@@ -1058,9 +1060,9 @@
       <c r="A55" s="9"/>
       <c r="B55" s="9"/>
       <c r="C55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="9"/>
       <c r="G55" s="9"/>
-      <c r="H55" s="9"/>
-      <c r="I55" s="9"/>
       <c r="J55" s="9"/>
       <c r="K55" s="9"/>
       <c r="L55" s="9"/>
@@ -1070,9 +1072,9 @@
       <c r="A56" s="9"/>
       <c r="B56" s="9"/>
       <c r="C56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="9"/>
       <c r="G56" s="9"/>
-      <c r="H56" s="9"/>
-      <c r="I56" s="9"/>
       <c r="J56" s="9"/>
       <c r="K56" s="9"/>
       <c r="L56" s="9"/>
@@ -1082,9 +1084,9 @@
       <c r="A57" s="9"/>
       <c r="B57" s="9"/>
       <c r="C57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="9"/>
       <c r="G57" s="9"/>
-      <c r="H57" s="9"/>
-      <c r="I57" s="9"/>
       <c r="J57" s="9"/>
       <c r="K57" s="9"/>
       <c r="L57" s="9"/>
@@ -1094,9 +1096,9 @@
       <c r="A58" s="9"/>
       <c r="B58" s="9"/>
       <c r="C58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="9"/>
       <c r="G58" s="9"/>
-      <c r="H58" s="9"/>
-      <c r="I58" s="9"/>
       <c r="J58" s="9"/>
       <c r="K58" s="9"/>
       <c r="L58" s="9"/>
@@ -1106,9 +1108,9 @@
       <c r="A59" s="9"/>
       <c r="B59" s="9"/>
       <c r="C59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="9"/>
       <c r="G59" s="9"/>
-      <c r="H59" s="9"/>
-      <c r="I59" s="9"/>
       <c r="J59" s="9"/>
       <c r="K59" s="9"/>
       <c r="L59" s="9"/>
@@ -1118,9 +1120,9 @@
       <c r="A60" s="9"/>
       <c r="B60" s="9"/>
       <c r="C60" s="9"/>
+      <c r="E60" s="9"/>
+      <c r="F60" s="9"/>
       <c r="G60" s="9"/>
-      <c r="H60" s="9"/>
-      <c r="I60" s="9"/>
       <c r="J60" s="9"/>
       <c r="K60" s="9"/>
       <c r="L60" s="9"/>
@@ -1130,9 +1132,9 @@
       <c r="A61" s="9"/>
       <c r="B61" s="9"/>
       <c r="C61" s="9"/>
+      <c r="E61" s="9"/>
+      <c r="F61" s="9"/>
       <c r="G61" s="9"/>
-      <c r="H61" s="9"/>
-      <c r="I61" s="9"/>
       <c r="J61" s="9"/>
       <c r="K61" s="9"/>
       <c r="L61" s="9"/>
@@ -1142,9 +1144,9 @@
       <c r="A62" s="9"/>
       <c r="B62" s="9"/>
       <c r="C62" s="9"/>
+      <c r="E62" s="9"/>
+      <c r="F62" s="9"/>
       <c r="G62" s="9"/>
-      <c r="H62" s="9"/>
-      <c r="I62" s="9"/>
       <c r="J62" s="9"/>
       <c r="K62" s="9"/>
       <c r="L62" s="9"/>
@@ -1154,9 +1156,9 @@
       <c r="A63" s="9"/>
       <c r="B63" s="9"/>
       <c r="C63" s="9"/>
+      <c r="E63" s="9"/>
+      <c r="F63" s="9"/>
       <c r="G63" s="9"/>
-      <c r="H63" s="9"/>
-      <c r="I63" s="9"/>
       <c r="J63" s="9"/>
       <c r="K63" s="9"/>
       <c r="L63" s="9"/>
@@ -1166,9 +1168,9 @@
       <c r="A64" s="9"/>
       <c r="B64" s="9"/>
       <c r="C64" s="9"/>
+      <c r="E64" s="9"/>
+      <c r="F64" s="9"/>
       <c r="G64" s="9"/>
-      <c r="H64" s="9"/>
-      <c r="I64" s="9"/>
       <c r="J64" s="9"/>
       <c r="K64" s="9"/>
       <c r="L64" s="9"/>
@@ -1178,9 +1180,9 @@
       <c r="A65" s="9"/>
       <c r="B65" s="9"/>
       <c r="C65" s="9"/>
+      <c r="E65" s="9"/>
+      <c r="F65" s="9"/>
       <c r="G65" s="9"/>
-      <c r="H65" s="9"/>
-      <c r="I65" s="9"/>
       <c r="J65" s="9"/>
       <c r="K65" s="9"/>
       <c r="L65" s="9"/>
@@ -1190,9 +1192,9 @@
       <c r="A66" s="9"/>
       <c r="B66" s="9"/>
       <c r="C66" s="9"/>
+      <c r="E66" s="9"/>
+      <c r="F66" s="9"/>
       <c r="G66" s="9"/>
-      <c r="H66" s="9"/>
-      <c r="I66" s="9"/>
       <c r="J66" s="9"/>
       <c r="K66" s="9"/>
       <c r="L66" s="9"/>
@@ -1202,9 +1204,9 @@
       <c r="A67" s="9"/>
       <c r="B67" s="9"/>
       <c r="C67" s="9"/>
+      <c r="E67" s="9"/>
+      <c r="F67" s="9"/>
       <c r="G67" s="9"/>
-      <c r="H67" s="9"/>
-      <c r="I67" s="9"/>
       <c r="J67" s="9"/>
       <c r="K67" s="9"/>
       <c r="L67" s="9"/>
@@ -1214,9 +1216,9 @@
       <c r="A68" s="9"/>
       <c r="B68" s="9"/>
       <c r="C68" s="9"/>
+      <c r="E68" s="9"/>
+      <c r="F68" s="9"/>
       <c r="G68" s="9"/>
-      <c r="H68" s="9"/>
-      <c r="I68" s="9"/>
       <c r="J68" s="9"/>
       <c r="K68" s="9"/>
       <c r="L68" s="9"/>
@@ -1226,9 +1228,9 @@
       <c r="A69" s="9"/>
       <c r="B69" s="9"/>
       <c r="C69" s="9"/>
+      <c r="E69" s="9"/>
+      <c r="F69" s="9"/>
       <c r="G69" s="9"/>
-      <c r="H69" s="9"/>
-      <c r="I69" s="9"/>
       <c r="J69" s="9"/>
       <c r="K69" s="9"/>
       <c r="L69" s="9"/>
@@ -1238,9 +1240,9 @@
       <c r="A70" s="9"/>
       <c r="B70" s="9"/>
       <c r="C70" s="9"/>
+      <c r="E70" s="9"/>
+      <c r="F70" s="9"/>
       <c r="G70" s="9"/>
-      <c r="H70" s="9"/>
-      <c r="I70" s="9"/>
       <c r="J70" s="9"/>
       <c r="K70" s="9"/>
       <c r="L70" s="9"/>
@@ -1250,9 +1252,9 @@
       <c r="A71" s="9"/>
       <c r="B71" s="9"/>
       <c r="C71" s="9"/>
+      <c r="E71" s="9"/>
+      <c r="F71" s="9"/>
       <c r="G71" s="9"/>
-      <c r="H71" s="9"/>
-      <c r="I71" s="9"/>
       <c r="J71" s="9"/>
       <c r="K71" s="9"/>
       <c r="L71" s="9"/>
@@ -1262,9 +1264,9 @@
       <c r="A72" s="9"/>
       <c r="B72" s="9"/>
       <c r="C72" s="9"/>
+      <c r="E72" s="9"/>
+      <c r="F72" s="9"/>
       <c r="G72" s="9"/>
-      <c r="H72" s="9"/>
-      <c r="I72" s="9"/>
       <c r="J72" s="9"/>
       <c r="K72" s="9"/>
       <c r="L72" s="9"/>
@@ -1274,9 +1276,9 @@
       <c r="A73" s="9"/>
       <c r="B73" s="9"/>
       <c r="C73" s="9"/>
+      <c r="E73" s="9"/>
+      <c r="F73" s="9"/>
       <c r="G73" s="9"/>
-      <c r="H73" s="9"/>
-      <c r="I73" s="9"/>
       <c r="J73" s="9"/>
       <c r="K73" s="9"/>
       <c r="L73" s="9"/>
@@ -1286,9 +1288,9 @@
       <c r="A74" s="9"/>
       <c r="B74" s="9"/>
       <c r="C74" s="9"/>
+      <c r="E74" s="9"/>
+      <c r="F74" s="9"/>
       <c r="G74" s="9"/>
-      <c r="H74" s="9"/>
-      <c r="I74" s="9"/>
       <c r="J74" s="9"/>
       <c r="K74" s="9"/>
       <c r="L74" s="9"/>
@@ -1298,9 +1300,9 @@
       <c r="A75" s="9"/>
       <c r="B75" s="9"/>
       <c r="C75" s="9"/>
+      <c r="E75" s="9"/>
+      <c r="F75" s="9"/>
       <c r="G75" s="9"/>
-      <c r="H75" s="9"/>
-      <c r="I75" s="9"/>
       <c r="J75" s="9"/>
       <c r="K75" s="9"/>
       <c r="L75" s="9"/>
@@ -1310,9 +1312,9 @@
       <c r="A76" s="9"/>
       <c r="B76" s="9"/>
       <c r="C76" s="9"/>
+      <c r="E76" s="9"/>
+      <c r="F76" s="9"/>
       <c r="G76" s="9"/>
-      <c r="H76" s="9"/>
-      <c r="I76" s="9"/>
       <c r="J76" s="9"/>
       <c r="K76" s="9"/>
       <c r="L76" s="9"/>
@@ -1322,9 +1324,9 @@
       <c r="A77" s="9"/>
       <c r="B77" s="9"/>
       <c r="C77" s="9"/>
+      <c r="E77" s="9"/>
+      <c r="F77" s="9"/>
       <c r="G77" s="9"/>
-      <c r="H77" s="9"/>
-      <c r="I77" s="9"/>
       <c r="J77" s="9"/>
       <c r="K77" s="9"/>
       <c r="L77" s="9"/>
@@ -1334,9 +1336,9 @@
       <c r="A78" s="9"/>
       <c r="B78" s="9"/>
       <c r="C78" s="9"/>
+      <c r="E78" s="9"/>
+      <c r="F78" s="9"/>
       <c r="G78" s="9"/>
-      <c r="H78" s="9"/>
-      <c r="I78" s="9"/>
       <c r="J78" s="9"/>
       <c r="K78" s="9"/>
       <c r="L78" s="9"/>
@@ -1346,9 +1348,9 @@
       <c r="A79" s="9"/>
       <c r="B79" s="9"/>
       <c r="C79" s="9"/>
+      <c r="E79" s="9"/>
+      <c r="F79" s="9"/>
       <c r="G79" s="9"/>
-      <c r="H79" s="9"/>
-      <c r="I79" s="9"/>
       <c r="J79" s="9"/>
       <c r="K79" s="9"/>
       <c r="L79" s="9"/>
@@ -1358,9 +1360,9 @@
       <c r="A80" s="9"/>
       <c r="B80" s="9"/>
       <c r="C80" s="9"/>
+      <c r="E80" s="9"/>
+      <c r="F80" s="9"/>
       <c r="G80" s="9"/>
-      <c r="H80" s="9"/>
-      <c r="I80" s="9"/>
       <c r="J80" s="9"/>
       <c r="K80" s="9"/>
       <c r="L80" s="9"/>
@@ -1370,9 +1372,9 @@
       <c r="A81" s="9"/>
       <c r="B81" s="9"/>
       <c r="C81" s="9"/>
+      <c r="E81" s="9"/>
+      <c r="F81" s="9"/>
       <c r="G81" s="9"/>
-      <c r="H81" s="9"/>
-      <c r="I81" s="9"/>
       <c r="J81" s="9"/>
       <c r="K81" s="9"/>
       <c r="L81" s="9"/>
@@ -1382,9 +1384,9 @@
       <c r="A82" s="9"/>
       <c r="B82" s="9"/>
       <c r="C82" s="9"/>
+      <c r="E82" s="9"/>
+      <c r="F82" s="9"/>
       <c r="G82" s="9"/>
-      <c r="H82" s="9"/>
-      <c r="I82" s="9"/>
       <c r="J82" s="9"/>
       <c r="K82" s="9"/>
       <c r="L82" s="9"/>
@@ -1394,9 +1396,9 @@
       <c r="A83" s="9"/>
       <c r="B83" s="9"/>
       <c r="C83" s="9"/>
+      <c r="E83" s="9"/>
+      <c r="F83" s="9"/>
       <c r="G83" s="9"/>
-      <c r="H83" s="9"/>
-      <c r="I83" s="9"/>
       <c r="J83" s="9"/>
       <c r="K83" s="9"/>
       <c r="L83" s="9"/>
@@ -1406,9 +1408,9 @@
       <c r="A84" s="9"/>
       <c r="B84" s="9"/>
       <c r="C84" s="9"/>
+      <c r="E84" s="9"/>
+      <c r="F84" s="9"/>
       <c r="G84" s="9"/>
-      <c r="H84" s="9"/>
-      <c r="I84" s="9"/>
       <c r="J84" s="9"/>
       <c r="K84" s="9"/>
       <c r="L84" s="9"/>
@@ -1418,9 +1420,9 @@
       <c r="A85" s="9"/>
       <c r="B85" s="9"/>
       <c r="C85" s="9"/>
+      <c r="E85" s="9"/>
+      <c r="F85" s="9"/>
       <c r="G85" s="9"/>
-      <c r="H85" s="9"/>
-      <c r="I85" s="9"/>
       <c r="J85" s="9"/>
       <c r="K85" s="9"/>
       <c r="L85" s="9"/>
@@ -1430,9 +1432,9 @@
       <c r="A86" s="9"/>
       <c r="B86" s="9"/>
       <c r="C86" s="9"/>
+      <c r="E86" s="9"/>
+      <c r="F86" s="9"/>
       <c r="G86" s="9"/>
-      <c r="H86" s="9"/>
-      <c r="I86" s="9"/>
       <c r="J86" s="9"/>
       <c r="K86" s="9"/>
       <c r="L86" s="9"/>
@@ -1442,9 +1444,9 @@
       <c r="A87" s="9"/>
       <c r="B87" s="9"/>
       <c r="C87" s="9"/>
+      <c r="E87" s="9"/>
+      <c r="F87" s="9"/>
       <c r="G87" s="9"/>
-      <c r="H87" s="9"/>
-      <c r="I87" s="9"/>
       <c r="J87" s="9"/>
       <c r="K87" s="9"/>
       <c r="L87" s="9"/>
@@ -1454,9 +1456,9 @@
       <c r="A88" s="9"/>
       <c r="B88" s="9"/>
       <c r="C88" s="9"/>
+      <c r="E88" s="9"/>
+      <c r="F88" s="9"/>
       <c r="G88" s="9"/>
-      <c r="H88" s="9"/>
-      <c r="I88" s="9"/>
       <c r="J88" s="9"/>
       <c r="K88" s="9"/>
       <c r="L88" s="9"/>
@@ -1466,9 +1468,9 @@
       <c r="A89" s="9"/>
       <c r="B89" s="9"/>
       <c r="C89" s="9"/>
+      <c r="E89" s="9"/>
+      <c r="F89" s="9"/>
       <c r="G89" s="9"/>
-      <c r="H89" s="9"/>
-      <c r="I89" s="9"/>
       <c r="J89" s="9"/>
       <c r="K89" s="9"/>
       <c r="L89" s="9"/>
@@ -1478,9 +1480,9 @@
       <c r="A90" s="9"/>
       <c r="B90" s="9"/>
       <c r="C90" s="9"/>
+      <c r="E90" s="9"/>
+      <c r="F90" s="9"/>
       <c r="G90" s="9"/>
-      <c r="H90" s="9"/>
-      <c r="I90" s="9"/>
       <c r="J90" s="9"/>
       <c r="K90" s="9"/>
       <c r="L90" s="9"/>
@@ -1490,9 +1492,9 @@
       <c r="A91" s="9"/>
       <c r="B91" s="9"/>
       <c r="C91" s="9"/>
+      <c r="E91" s="9"/>
+      <c r="F91" s="9"/>
       <c r="G91" s="9"/>
-      <c r="H91" s="9"/>
-      <c r="I91" s="9"/>
       <c r="J91" s="9"/>
       <c r="K91" s="9"/>
       <c r="L91" s="9"/>
@@ -1502,9 +1504,9 @@
       <c r="A92" s="9"/>
       <c r="B92" s="9"/>
       <c r="C92" s="9"/>
+      <c r="E92" s="9"/>
+      <c r="F92" s="9"/>
       <c r="G92" s="9"/>
-      <c r="H92" s="9"/>
-      <c r="I92" s="9"/>
       <c r="J92" s="9"/>
       <c r="K92" s="9"/>
       <c r="L92" s="9"/>
@@ -1514,9 +1516,9 @@
       <c r="A93" s="9"/>
       <c r="B93" s="9"/>
       <c r="C93" s="9"/>
+      <c r="E93" s="9"/>
+      <c r="F93" s="9"/>
       <c r="G93" s="9"/>
-      <c r="H93" s="9"/>
-      <c r="I93" s="9"/>
       <c r="J93" s="9"/>
       <c r="K93" s="9"/>
       <c r="L93" s="9"/>
@@ -1526,9 +1528,9 @@
       <c r="A94" s="9"/>
       <c r="B94" s="9"/>
       <c r="C94" s="9"/>
+      <c r="E94" s="9"/>
+      <c r="F94" s="9"/>
       <c r="G94" s="9"/>
-      <c r="H94" s="9"/>
-      <c r="I94" s="9"/>
       <c r="J94" s="9"/>
       <c r="K94" s="9"/>
       <c r="L94" s="9"/>
@@ -1538,9 +1540,9 @@
       <c r="A95" s="9"/>
       <c r="B95" s="9"/>
       <c r="C95" s="9"/>
+      <c r="E95" s="9"/>
+      <c r="F95" s="9"/>
       <c r="G95" s="9"/>
-      <c r="H95" s="9"/>
-      <c r="I95" s="9"/>
       <c r="J95" s="9"/>
       <c r="K95" s="9"/>
       <c r="L95" s="9"/>
@@ -1550,9 +1552,9 @@
       <c r="A96" s="9"/>
       <c r="B96" s="9"/>
       <c r="C96" s="9"/>
+      <c r="E96" s="9"/>
+      <c r="F96" s="9"/>
       <c r="G96" s="9"/>
-      <c r="H96" s="9"/>
-      <c r="I96" s="9"/>
       <c r="J96" s="9"/>
       <c r="K96" s="9"/>
       <c r="L96" s="9"/>
@@ -1562,9 +1564,9 @@
       <c r="A97" s="9"/>
       <c r="B97" s="9"/>
       <c r="C97" s="9"/>
+      <c r="E97" s="9"/>
+      <c r="F97" s="9"/>
       <c r="G97" s="9"/>
-      <c r="H97" s="9"/>
-      <c r="I97" s="9"/>
       <c r="J97" s="9"/>
       <c r="K97" s="9"/>
       <c r="L97" s="9"/>
@@ -1574,9 +1576,9 @@
       <c r="A98" s="9"/>
       <c r="B98" s="9"/>
       <c r="C98" s="9"/>
+      <c r="E98" s="9"/>
+      <c r="F98" s="9"/>
       <c r="G98" s="9"/>
-      <c r="H98" s="9"/>
-      <c r="I98" s="9"/>
       <c r="J98" s="9"/>
       <c r="K98" s="9"/>
       <c r="L98" s="9"/>
@@ -1586,9 +1588,9 @@
       <c r="A99" s="9"/>
       <c r="B99" s="9"/>
       <c r="C99" s="9"/>
+      <c r="E99" s="9"/>
+      <c r="F99" s="9"/>
       <c r="G99" s="9"/>
-      <c r="H99" s="9"/>
-      <c r="I99" s="9"/>
       <c r="J99" s="9"/>
       <c r="K99" s="9"/>
       <c r="L99" s="9"/>
@@ -1598,9 +1600,9 @@
       <c r="A100" s="9"/>
       <c r="B100" s="9"/>
       <c r="C100" s="9"/>
+      <c r="E100" s="9"/>
+      <c r="F100" s="9"/>
       <c r="G100" s="9"/>
-      <c r="H100" s="9"/>
-      <c r="I100" s="9"/>
       <c r="J100" s="9"/>
       <c r="K100" s="9"/>
       <c r="L100" s="9"/>
@@ -1610,9 +1612,9 @@
       <c r="A101" s="9"/>
       <c r="B101" s="9"/>
       <c r="C101" s="9"/>
+      <c r="E101" s="9"/>
+      <c r="F101" s="9"/>
       <c r="G101" s="9"/>
-      <c r="H101" s="9"/>
-      <c r="I101" s="9"/>
       <c r="J101" s="9"/>
       <c r="K101" s="9"/>
       <c r="L101" s="9"/>
@@ -1622,9 +1624,9 @@
       <c r="A102" s="9"/>
       <c r="B102" s="9"/>
       <c r="C102" s="9"/>
+      <c r="E102" s="9"/>
+      <c r="F102" s="9"/>
       <c r="G102" s="9"/>
-      <c r="H102" s="9"/>
-      <c r="I102" s="9"/>
       <c r="J102" s="9"/>
       <c r="K102" s="9"/>
       <c r="L102" s="9"/>
@@ -1634,9 +1636,9 @@
       <c r="A103" s="9"/>
       <c r="B103" s="9"/>
       <c r="C103" s="9"/>
+      <c r="E103" s="9"/>
+      <c r="F103" s="9"/>
       <c r="G103" s="9"/>
-      <c r="H103" s="9"/>
-      <c r="I103" s="9"/>
       <c r="J103" s="9"/>
       <c r="K103" s="9"/>
       <c r="L103" s="9"/>
@@ -1646,9 +1648,9 @@
       <c r="A104" s="9"/>
       <c r="B104" s="9"/>
       <c r="C104" s="9"/>
+      <c r="E104" s="9"/>
+      <c r="F104" s="9"/>
       <c r="G104" s="9"/>
-      <c r="H104" s="9"/>
-      <c r="I104" s="9"/>
       <c r="J104" s="9"/>
       <c r="K104" s="9"/>
       <c r="L104" s="9"/>
@@ -1658,9 +1660,9 @@
       <c r="A105" s="9"/>
       <c r="B105" s="9"/>
       <c r="C105" s="9"/>
+      <c r="E105" s="9"/>
+      <c r="F105" s="9"/>
       <c r="G105" s="9"/>
-      <c r="H105" s="9"/>
-      <c r="I105" s="9"/>
       <c r="J105" s="9"/>
       <c r="K105" s="9"/>
       <c r="L105" s="9"/>
@@ -1670,9 +1672,9 @@
       <c r="A106" s="9"/>
       <c r="B106" s="9"/>
       <c r="C106" s="9"/>
+      <c r="E106" s="9"/>
+      <c r="F106" s="9"/>
       <c r="G106" s="9"/>
-      <c r="H106" s="9"/>
-      <c r="I106" s="9"/>
       <c r="J106" s="9"/>
       <c r="K106" s="9"/>
       <c r="L106" s="9"/>
@@ -1682,9 +1684,9 @@
       <c r="A107" s="9"/>
       <c r="B107" s="9"/>
       <c r="C107" s="9"/>
+      <c r="E107" s="9"/>
+      <c r="F107" s="9"/>
       <c r="G107" s="9"/>
-      <c r="H107" s="9"/>
-      <c r="I107" s="9"/>
       <c r="J107" s="9"/>
       <c r="K107" s="9"/>
       <c r="L107" s="9"/>
@@ -1694,9 +1696,9 @@
       <c r="A108" s="9"/>
       <c r="B108" s="9"/>
       <c r="C108" s="9"/>
+      <c r="E108" s="9"/>
+      <c r="F108" s="9"/>
       <c r="G108" s="9"/>
-      <c r="H108" s="9"/>
-      <c r="I108" s="9"/>
       <c r="J108" s="9"/>
       <c r="K108" s="9"/>
       <c r="L108" s="9"/>
@@ -1706,9 +1708,9 @@
       <c r="A109" s="9"/>
       <c r="B109" s="9"/>
       <c r="C109" s="9"/>
+      <c r="E109" s="9"/>
+      <c r="F109" s="9"/>
       <c r="G109" s="9"/>
-      <c r="H109" s="9"/>
-      <c r="I109" s="9"/>
       <c r="J109" s="9"/>
       <c r="K109" s="9"/>
       <c r="L109" s="9"/>
@@ -1718,9 +1720,9 @@
       <c r="A110" s="9"/>
       <c r="B110" s="9"/>
       <c r="C110" s="9"/>
+      <c r="E110" s="9"/>
+      <c r="F110" s="9"/>
       <c r="G110" s="9"/>
-      <c r="H110" s="9"/>
-      <c r="I110" s="9"/>
       <c r="J110" s="9"/>
       <c r="K110" s="9"/>
       <c r="L110" s="9"/>
@@ -1730,9 +1732,9 @@
       <c r="A111" s="9"/>
       <c r="B111" s="9"/>
       <c r="C111" s="9"/>
+      <c r="E111" s="9"/>
+      <c r="F111" s="9"/>
       <c r="G111" s="9"/>
-      <c r="H111" s="9"/>
-      <c r="I111" s="9"/>
       <c r="J111" s="9"/>
       <c r="K111" s="9"/>
       <c r="L111" s="9"/>
@@ -1742,9 +1744,9 @@
       <c r="A112" s="9"/>
       <c r="B112" s="9"/>
       <c r="C112" s="9"/>
+      <c r="E112" s="9"/>
+      <c r="F112" s="9"/>
       <c r="G112" s="9"/>
-      <c r="H112" s="9"/>
-      <c r="I112" s="9"/>
       <c r="J112" s="9"/>
       <c r="K112" s="9"/>
       <c r="L112" s="9"/>
@@ -1754,9 +1756,9 @@
       <c r="A113" s="9"/>
       <c r="B113" s="9"/>
       <c r="C113" s="9"/>
+      <c r="E113" s="9"/>
+      <c r="F113" s="9"/>
       <c r="G113" s="9"/>
-      <c r="H113" s="9"/>
-      <c r="I113" s="9"/>
       <c r="J113" s="9"/>
       <c r="K113" s="9"/>
       <c r="L113" s="9"/>
@@ -1766,9 +1768,9 @@
       <c r="A114" s="9"/>
       <c r="B114" s="9"/>
       <c r="C114" s="9"/>
+      <c r="E114" s="9"/>
+      <c r="F114" s="9"/>
       <c r="G114" s="9"/>
-      <c r="H114" s="9"/>
-      <c r="I114" s="9"/>
       <c r="J114" s="9"/>
       <c r="K114" s="9"/>
       <c r="L114" s="9"/>
@@ -1778,9 +1780,9 @@
       <c r="A115" s="9"/>
       <c r="B115" s="9"/>
       <c r="C115" s="9"/>
+      <c r="E115" s="9"/>
+      <c r="F115" s="9"/>
       <c r="G115" s="9"/>
-      <c r="H115" s="9"/>
-      <c r="I115" s="9"/>
       <c r="J115" s="9"/>
       <c r="K115" s="9"/>
       <c r="L115" s="9"/>
@@ -1790,9 +1792,9 @@
       <c r="A116" s="9"/>
       <c r="B116" s="9"/>
       <c r="C116" s="9"/>
+      <c r="E116" s="9"/>
+      <c r="F116" s="9"/>
       <c r="G116" s="9"/>
-      <c r="H116" s="9"/>
-      <c r="I116" s="9"/>
       <c r="J116" s="9"/>
       <c r="K116" s="9"/>
       <c r="L116" s="9"/>
@@ -1802,9 +1804,9 @@
       <c r="A117" s="9"/>
       <c r="B117" s="9"/>
       <c r="C117" s="9"/>
+      <c r="E117" s="9"/>
+      <c r="F117" s="9"/>
       <c r="G117" s="9"/>
-      <c r="H117" s="9"/>
-      <c r="I117" s="9"/>
       <c r="J117" s="9"/>
       <c r="K117" s="9"/>
       <c r="L117" s="9"/>
@@ -1814,9 +1816,9 @@
       <c r="A118" s="9"/>
       <c r="B118" s="9"/>
       <c r="C118" s="9"/>
+      <c r="E118" s="9"/>
+      <c r="F118" s="9"/>
       <c r="G118" s="9"/>
-      <c r="H118" s="9"/>
-      <c r="I118" s="9"/>
       <c r="J118" s="9"/>
       <c r="K118" s="9"/>
       <c r="L118" s="9"/>
@@ -1826,9 +1828,9 @@
       <c r="A119" s="9"/>
       <c r="B119" s="9"/>
       <c r="C119" s="9"/>
+      <c r="E119" s="9"/>
+      <c r="F119" s="9"/>
       <c r="G119" s="9"/>
-      <c r="H119" s="9"/>
-      <c r="I119" s="9"/>
       <c r="J119" s="9"/>
       <c r="K119" s="9"/>
       <c r="L119" s="9"/>
@@ -1838,9 +1840,9 @@
       <c r="A120" s="9"/>
       <c r="B120" s="9"/>
       <c r="C120" s="9"/>
+      <c r="E120" s="9"/>
+      <c r="F120" s="9"/>
       <c r="G120" s="9"/>
-      <c r="H120" s="9"/>
-      <c r="I120" s="9"/>
       <c r="J120" s="9"/>
       <c r="K120" s="9"/>
       <c r="L120" s="9"/>
@@ -1850,9 +1852,9 @@
       <c r="A121" s="9"/>
       <c r="B121" s="9"/>
       <c r="C121" s="9"/>
+      <c r="E121" s="9"/>
+      <c r="F121" s="9"/>
       <c r="G121" s="9"/>
-      <c r="H121" s="9"/>
-      <c r="I121" s="9"/>
       <c r="J121" s="9"/>
       <c r="K121" s="9"/>
       <c r="L121" s="9"/>
@@ -1862,9 +1864,9 @@
       <c r="A122" s="9"/>
       <c r="B122" s="9"/>
       <c r="C122" s="9"/>
+      <c r="E122" s="9"/>
+      <c r="F122" s="9"/>
       <c r="G122" s="9"/>
-      <c r="H122" s="9"/>
-      <c r="I122" s="9"/>
       <c r="J122" s="9"/>
       <c r="K122" s="9"/>
       <c r="L122" s="9"/>
@@ -1874,9 +1876,9 @@
       <c r="A123" s="9"/>
       <c r="B123" s="9"/>
       <c r="C123" s="9"/>
+      <c r="E123" s="9"/>
+      <c r="F123" s="9"/>
       <c r="G123" s="9"/>
-      <c r="H123" s="9"/>
-      <c r="I123" s="9"/>
       <c r="J123" s="9"/>
       <c r="K123" s="9"/>
       <c r="L123" s="9"/>
@@ -1886,9 +1888,9 @@
       <c r="A124" s="9"/>
       <c r="B124" s="9"/>
       <c r="C124" s="9"/>
+      <c r="E124" s="9"/>
+      <c r="F124" s="9"/>
       <c r="G124" s="9"/>
-      <c r="H124" s="9"/>
-      <c r="I124" s="9"/>
       <c r="J124" s="9"/>
       <c r="K124" s="9"/>
       <c r="L124" s="9"/>
@@ -1898,9 +1900,9 @@
       <c r="A125" s="9"/>
       <c r="B125" s="9"/>
       <c r="C125" s="9"/>
+      <c r="E125" s="9"/>
+      <c r="F125" s="9"/>
       <c r="G125" s="9"/>
-      <c r="H125" s="9"/>
-      <c r="I125" s="9"/>
       <c r="J125" s="9"/>
       <c r="K125" s="9"/>
       <c r="L125" s="9"/>
@@ -1910,9 +1912,9 @@
       <c r="A126" s="9"/>
       <c r="B126" s="9"/>
       <c r="C126" s="9"/>
+      <c r="E126" s="9"/>
+      <c r="F126" s="9"/>
       <c r="G126" s="9"/>
-      <c r="H126" s="9"/>
-      <c r="I126" s="9"/>
       <c r="J126" s="9"/>
       <c r="K126" s="9"/>
       <c r="L126" s="9"/>
@@ -1922,9 +1924,9 @@
       <c r="A127" s="9"/>
       <c r="B127" s="9"/>
       <c r="C127" s="9"/>
+      <c r="E127" s="9"/>
+      <c r="F127" s="9"/>
       <c r="G127" s="9"/>
-      <c r="H127" s="9"/>
-      <c r="I127" s="9"/>
       <c r="J127" s="9"/>
       <c r="K127" s="9"/>
       <c r="L127" s="9"/>
@@ -1934,9 +1936,9 @@
       <c r="A128" s="9"/>
       <c r="B128" s="9"/>
       <c r="C128" s="9"/>
+      <c r="E128" s="9"/>
+      <c r="F128" s="9"/>
       <c r="G128" s="9"/>
-      <c r="H128" s="9"/>
-      <c r="I128" s="9"/>
       <c r="J128" s="9"/>
       <c r="K128" s="9"/>
       <c r="L128" s="9"/>
@@ -1946,9 +1948,9 @@
       <c r="A129" s="9"/>
       <c r="B129" s="9"/>
       <c r="C129" s="9"/>
+      <c r="E129" s="9"/>
+      <c r="F129" s="9"/>
       <c r="G129" s="9"/>
-      <c r="H129" s="9"/>
-      <c r="I129" s="9"/>
       <c r="J129" s="9"/>
       <c r="K129" s="9"/>
       <c r="L129" s="9"/>
@@ -1958,9 +1960,9 @@
       <c r="A130" s="9"/>
       <c r="B130" s="9"/>
       <c r="C130" s="9"/>
+      <c r="E130" s="9"/>
+      <c r="F130" s="9"/>
       <c r="G130" s="9"/>
-      <c r="H130" s="9"/>
-      <c r="I130" s="9"/>
       <c r="J130" s="9"/>
       <c r="K130" s="9"/>
       <c r="L130" s="9"/>
@@ -1970,9 +1972,9 @@
       <c r="A131" s="9"/>
       <c r="B131" s="9"/>
       <c r="C131" s="9"/>
+      <c r="E131" s="9"/>
+      <c r="F131" s="9"/>
       <c r="G131" s="9"/>
-      <c r="H131" s="9"/>
-      <c r="I131" s="9"/>
       <c r="J131" s="9"/>
       <c r="K131" s="9"/>
       <c r="L131" s="9"/>
@@ -1982,9 +1984,9 @@
       <c r="A132" s="9"/>
       <c r="B132" s="9"/>
       <c r="C132" s="9"/>
+      <c r="E132" s="9"/>
+      <c r="F132" s="9"/>
       <c r="G132" s="9"/>
-      <c r="H132" s="9"/>
-      <c r="I132" s="9"/>
       <c r="J132" s="9"/>
       <c r="K132" s="9"/>
       <c r="L132" s="9"/>
@@ -1994,9 +1996,9 @@
       <c r="A133" s="9"/>
       <c r="B133" s="9"/>
       <c r="C133" s="9"/>
+      <c r="E133" s="9"/>
+      <c r="F133" s="9"/>
       <c r="G133" s="9"/>
-      <c r="H133" s="9"/>
-      <c r="I133" s="9"/>
       <c r="J133" s="9"/>
       <c r="K133" s="9"/>
       <c r="L133" s="9"/>
@@ -2006,9 +2008,9 @@
       <c r="A134" s="9"/>
       <c r="B134" s="9"/>
       <c r="C134" s="9"/>
+      <c r="E134" s="9"/>
+      <c r="F134" s="9"/>
       <c r="G134" s="9"/>
-      <c r="H134" s="9"/>
-      <c r="I134" s="9"/>
       <c r="J134" s="9"/>
       <c r="K134" s="9"/>
       <c r="L134" s="9"/>
@@ -2018,9 +2020,9 @@
       <c r="A135" s="9"/>
       <c r="B135" s="9"/>
       <c r="C135" s="9"/>
+      <c r="E135" s="9"/>
+      <c r="F135" s="9"/>
       <c r="G135" s="9"/>
-      <c r="H135" s="9"/>
-      <c r="I135" s="9"/>
       <c r="J135" s="9"/>
       <c r="K135" s="9"/>
       <c r="L135" s="9"/>
@@ -2030,9 +2032,9 @@
       <c r="A136" s="9"/>
       <c r="B136" s="9"/>
       <c r="C136" s="9"/>
+      <c r="E136" s="9"/>
+      <c r="F136" s="9"/>
       <c r="G136" s="9"/>
-      <c r="H136" s="9"/>
-      <c r="I136" s="9"/>
       <c r="J136" s="9"/>
       <c r="K136" s="9"/>
       <c r="L136" s="9"/>
@@ -2042,9 +2044,9 @@
       <c r="A137" s="9"/>
       <c r="B137" s="9"/>
       <c r="C137" s="9"/>
+      <c r="E137" s="9"/>
+      <c r="F137" s="9"/>
       <c r="G137" s="9"/>
-      <c r="H137" s="9"/>
-      <c r="I137" s="9"/>
       <c r="J137" s="9"/>
       <c r="K137" s="9"/>
       <c r="L137" s="9"/>
@@ -2054,9 +2056,9 @@
       <c r="A138" s="9"/>
       <c r="B138" s="9"/>
       <c r="C138" s="9"/>
+      <c r="E138" s="9"/>
+      <c r="F138" s="9"/>
       <c r="G138" s="9"/>
-      <c r="H138" s="9"/>
-      <c r="I138" s="9"/>
       <c r="J138" s="9"/>
       <c r="K138" s="9"/>
       <c r="L138" s="9"/>
@@ -2066,9 +2068,9 @@
       <c r="A139" s="9"/>
       <c r="B139" s="9"/>
       <c r="C139" s="9"/>
+      <c r="E139" s="9"/>
+      <c r="F139" s="9"/>
       <c r="G139" s="9"/>
-      <c r="H139" s="9"/>
-      <c r="I139" s="9"/>
       <c r="J139" s="9"/>
       <c r="K139" s="9"/>
       <c r="L139" s="9"/>
@@ -2078,9 +2080,9 @@
       <c r="A140" s="9"/>
       <c r="B140" s="9"/>
       <c r="C140" s="9"/>
+      <c r="E140" s="9"/>
+      <c r="F140" s="9"/>
       <c r="G140" s="9"/>
-      <c r="H140" s="9"/>
-      <c r="I140" s="9"/>
       <c r="J140" s="9"/>
       <c r="K140" s="9"/>
       <c r="L140" s="9"/>
@@ -2090,9 +2092,9 @@
       <c r="A141" s="9"/>
       <c r="B141" s="9"/>
       <c r="C141" s="9"/>
+      <c r="E141" s="9"/>
+      <c r="F141" s="9"/>
       <c r="G141" s="9"/>
-      <c r="H141" s="9"/>
-      <c r="I141" s="9"/>
       <c r="J141" s="9"/>
       <c r="K141" s="9"/>
       <c r="L141" s="9"/>
@@ -2102,9 +2104,9 @@
       <c r="A142" s="9"/>
       <c r="B142" s="9"/>
       <c r="C142" s="9"/>
+      <c r="E142" s="9"/>
+      <c r="F142" s="9"/>
       <c r="G142" s="9"/>
-      <c r="H142" s="9"/>
-      <c r="I142" s="9"/>
       <c r="J142" s="9"/>
       <c r="K142" s="9"/>
       <c r="L142" s="9"/>
@@ -2114,9 +2116,9 @@
       <c r="A143" s="9"/>
       <c r="B143" s="9"/>
       <c r="C143" s="9"/>
+      <c r="E143" s="9"/>
+      <c r="F143" s="9"/>
       <c r="G143" s="9"/>
-      <c r="H143" s="9"/>
-      <c r="I143" s="9"/>
       <c r="J143" s="9"/>
       <c r="K143" s="9"/>
       <c r="L143" s="9"/>
@@ -2126,9 +2128,9 @@
       <c r="A144" s="9"/>
       <c r="B144" s="9"/>
       <c r="C144" s="9"/>
+      <c r="E144" s="9"/>
+      <c r="F144" s="9"/>
       <c r="G144" s="9"/>
-      <c r="H144" s="9"/>
-      <c r="I144" s="9"/>
       <c r="J144" s="9"/>
       <c r="K144" s="9"/>
       <c r="L144" s="9"/>
@@ -2138,9 +2140,9 @@
       <c r="A145" s="9"/>
       <c r="B145" s="9"/>
       <c r="C145" s="9"/>
+      <c r="E145" s="9"/>
+      <c r="F145" s="9"/>
       <c r="G145" s="9"/>
-      <c r="H145" s="9"/>
-      <c r="I145" s="9"/>
       <c r="J145" s="9"/>
       <c r="K145" s="9"/>
       <c r="L145" s="9"/>
@@ -2150,9 +2152,9 @@
       <c r="A146" s="9"/>
       <c r="B146" s="9"/>
       <c r="C146" s="9"/>
+      <c r="E146" s="9"/>
+      <c r="F146" s="9"/>
       <c r="G146" s="9"/>
-      <c r="H146" s="9"/>
-      <c r="I146" s="9"/>
       <c r="J146" s="9"/>
       <c r="K146" s="9"/>
       <c r="L146" s="9"/>
@@ -2162,9 +2164,9 @@
       <c r="A147" s="9"/>
       <c r="B147" s="9"/>
       <c r="C147" s="9"/>
+      <c r="E147" s="9"/>
+      <c r="F147" s="9"/>
       <c r="G147" s="9"/>
-      <c r="H147" s="9"/>
-      <c r="I147" s="9"/>
       <c r="J147" s="9"/>
       <c r="K147" s="9"/>
       <c r="L147" s="9"/>
@@ -2174,9 +2176,9 @@
       <c r="A148" s="9"/>
       <c r="B148" s="9"/>
       <c r="C148" s="9"/>
+      <c r="E148" s="9"/>
+      <c r="F148" s="9"/>
       <c r="G148" s="9"/>
-      <c r="H148" s="9"/>
-      <c r="I148" s="9"/>
       <c r="J148" s="9"/>
       <c r="K148" s="9"/>
       <c r="L148" s="9"/>
@@ -2186,9 +2188,9 @@
       <c r="A149" s="9"/>
       <c r="B149" s="9"/>
       <c r="C149" s="9"/>
+      <c r="E149" s="9"/>
+      <c r="F149" s="9"/>
       <c r="G149" s="9"/>
-      <c r="H149" s="9"/>
-      <c r="I149" s="9"/>
       <c r="J149" s="9"/>
       <c r="K149" s="9"/>
       <c r="L149" s="9"/>
@@ -2198,9 +2200,9 @@
       <c r="A150" s="9"/>
       <c r="B150" s="9"/>
       <c r="C150" s="9"/>
+      <c r="E150" s="9"/>
+      <c r="F150" s="9"/>
       <c r="G150" s="9"/>
-      <c r="H150" s="9"/>
-      <c r="I150" s="9"/>
       <c r="J150" s="9"/>
       <c r="K150" s="9"/>
       <c r="L150" s="9"/>
@@ -2210,9 +2212,9 @@
       <c r="A151" s="9"/>
       <c r="B151" s="9"/>
       <c r="C151" s="9"/>
+      <c r="E151" s="9"/>
+      <c r="F151" s="9"/>
       <c r="G151" s="9"/>
-      <c r="H151" s="9"/>
-      <c r="I151" s="9"/>
       <c r="J151" s="9"/>
       <c r="K151" s="9"/>
       <c r="L151" s="9"/>
@@ -2222,9 +2224,9 @@
       <c r="A152" s="9"/>
       <c r="B152" s="9"/>
       <c r="C152" s="9"/>
+      <c r="E152" s="9"/>
+      <c r="F152" s="9"/>
       <c r="G152" s="9"/>
-      <c r="H152" s="9"/>
-      <c r="I152" s="9"/>
       <c r="J152" s="9"/>
       <c r="K152" s="9"/>
       <c r="L152" s="9"/>
@@ -2234,9 +2236,9 @@
       <c r="A153" s="9"/>
       <c r="B153" s="9"/>
       <c r="C153" s="9"/>
+      <c r="E153" s="9"/>
+      <c r="F153" s="9"/>
       <c r="G153" s="9"/>
-      <c r="H153" s="9"/>
-      <c r="I153" s="9"/>
       <c r="J153" s="9"/>
       <c r="K153" s="9"/>
       <c r="L153" s="9"/>
@@ -2246,9 +2248,9 @@
       <c r="A154" s="9"/>
       <c r="B154" s="9"/>
       <c r="C154" s="9"/>
+      <c r="E154" s="9"/>
+      <c r="F154" s="9"/>
       <c r="G154" s="9"/>
-      <c r="H154" s="9"/>
-      <c r="I154" s="9"/>
       <c r="J154" s="9"/>
       <c r="K154" s="9"/>
       <c r="L154" s="9"/>
@@ -2258,9 +2260,9 @@
       <c r="A155" s="9"/>
       <c r="B155" s="9"/>
       <c r="C155" s="9"/>
+      <c r="E155" s="9"/>
+      <c r="F155" s="9"/>
       <c r="G155" s="9"/>
-      <c r="H155" s="9"/>
-      <c r="I155" s="9"/>
       <c r="J155" s="9"/>
       <c r="K155" s="9"/>
       <c r="L155" s="9"/>
@@ -2270,9 +2272,9 @@
       <c r="A156" s="9"/>
       <c r="B156" s="9"/>
       <c r="C156" s="9"/>
+      <c r="E156" s="9"/>
+      <c r="F156" s="9"/>
       <c r="G156" s="9"/>
-      <c r="H156" s="9"/>
-      <c r="I156" s="9"/>
       <c r="J156" s="9"/>
       <c r="K156" s="9"/>
       <c r="L156" s="9"/>
@@ -2282,9 +2284,9 @@
       <c r="A157" s="9"/>
       <c r="B157" s="9"/>
       <c r="C157" s="9"/>
+      <c r="E157" s="9"/>
+      <c r="F157" s="9"/>
       <c r="G157" s="9"/>
-      <c r="H157" s="9"/>
-      <c r="I157" s="9"/>
       <c r="J157" s="9"/>
       <c r="K157" s="9"/>
       <c r="L157" s="9"/>
@@ -2294,9 +2296,9 @@
       <c r="A158" s="9"/>
       <c r="B158" s="9"/>
       <c r="C158" s="9"/>
+      <c r="E158" s="9"/>
+      <c r="F158" s="9"/>
       <c r="G158" s="9"/>
-      <c r="H158" s="9"/>
-      <c r="I158" s="9"/>
       <c r="J158" s="9"/>
       <c r="K158" s="9"/>
       <c r="L158" s="9"/>
@@ -2306,9 +2308,9 @@
       <c r="A159" s="9"/>
       <c r="B159" s="9"/>
       <c r="C159" s="9"/>
+      <c r="E159" s="9"/>
+      <c r="F159" s="9"/>
       <c r="G159" s="9"/>
-      <c r="H159" s="9"/>
-      <c r="I159" s="9"/>
       <c r="J159" s="9"/>
       <c r="K159" s="9"/>
       <c r="L159" s="9"/>
@@ -2318,9 +2320,9 @@
       <c r="A160" s="9"/>
       <c r="B160" s="9"/>
       <c r="C160" s="9"/>
+      <c r="E160" s="9"/>
+      <c r="F160" s="9"/>
       <c r="G160" s="9"/>
-      <c r="H160" s="9"/>
-      <c r="I160" s="9"/>
       <c r="J160" s="9"/>
       <c r="K160" s="9"/>
       <c r="L160" s="9"/>
@@ -2330,9 +2332,9 @@
       <c r="A161" s="9"/>
       <c r="B161" s="9"/>
       <c r="C161" s="9"/>
+      <c r="E161" s="9"/>
+      <c r="F161" s="9"/>
       <c r="G161" s="9"/>
-      <c r="H161" s="9"/>
-      <c r="I161" s="9"/>
       <c r="J161" s="9"/>
       <c r="K161" s="9"/>
       <c r="L161" s="9"/>
@@ -2342,9 +2344,9 @@
       <c r="A162" s="9"/>
       <c r="B162" s="9"/>
       <c r="C162" s="9"/>
+      <c r="E162" s="9"/>
+      <c r="F162" s="9"/>
       <c r="G162" s="9"/>
-      <c r="H162" s="9"/>
-      <c r="I162" s="9"/>
       <c r="J162" s="9"/>
       <c r="K162" s="9"/>
       <c r="L162" s="9"/>
@@ -2354,9 +2356,9 @@
       <c r="A163" s="9"/>
       <c r="B163" s="9"/>
       <c r="C163" s="9"/>
+      <c r="E163" s="9"/>
+      <c r="F163" s="9"/>
       <c r="G163" s="9"/>
-      <c r="H163" s="9"/>
-      <c r="I163" s="9"/>
       <c r="J163" s="9"/>
       <c r="K163" s="9"/>
       <c r="L163" s="9"/>
@@ -2366,9 +2368,9 @@
       <c r="A164" s="9"/>
       <c r="B164" s="9"/>
       <c r="C164" s="9"/>
+      <c r="E164" s="9"/>
+      <c r="F164" s="9"/>
       <c r="G164" s="9"/>
-      <c r="H164" s="9"/>
-      <c r="I164" s="9"/>
       <c r="J164" s="9"/>
       <c r="K164" s="9"/>
       <c r="L164" s="9"/>
@@ -2378,9 +2380,9 @@
       <c r="A165" s="9"/>
       <c r="B165" s="9"/>
       <c r="C165" s="9"/>
+      <c r="E165" s="9"/>
+      <c r="F165" s="9"/>
       <c r="G165" s="9"/>
-      <c r="H165" s="9"/>
-      <c r="I165" s="9"/>
       <c r="J165" s="9"/>
       <c r="K165" s="9"/>
       <c r="L165" s="9"/>
@@ -2390,9 +2392,9 @@
       <c r="A166" s="9"/>
       <c r="B166" s="9"/>
       <c r="C166" s="9"/>
+      <c r="E166" s="9"/>
+      <c r="F166" s="9"/>
       <c r="G166" s="9"/>
-      <c r="H166" s="9"/>
-      <c r="I166" s="9"/>
       <c r="J166" s="9"/>
       <c r="K166" s="9"/>
       <c r="L166" s="9"/>
@@ -2402,9 +2404,9 @@
       <c r="A167" s="9"/>
       <c r="B167" s="9"/>
       <c r="C167" s="9"/>
+      <c r="E167" s="9"/>
+      <c r="F167" s="9"/>
       <c r="G167" s="9"/>
-      <c r="H167" s="9"/>
-      <c r="I167" s="9"/>
       <c r="J167" s="9"/>
       <c r="K167" s="9"/>
       <c r="L167" s="9"/>
@@ -2414,9 +2416,9 @@
       <c r="A168" s="9"/>
       <c r="B168" s="9"/>
       <c r="C168" s="9"/>
+      <c r="E168" s="9"/>
+      <c r="F168" s="9"/>
       <c r="G168" s="9"/>
-      <c r="H168" s="9"/>
-      <c r="I168" s="9"/>
       <c r="J168" s="9"/>
       <c r="K168" s="9"/>
       <c r="L168" s="9"/>
@@ -2426,9 +2428,9 @@
       <c r="A169" s="9"/>
       <c r="B169" s="9"/>
       <c r="C169" s="9"/>
+      <c r="E169" s="9"/>
+      <c r="F169" s="9"/>
       <c r="G169" s="9"/>
-      <c r="H169" s="9"/>
-      <c r="I169" s="9"/>
       <c r="J169" s="9"/>
       <c r="K169" s="9"/>
       <c r="L169" s="9"/>
@@ -2438,9 +2440,9 @@
       <c r="A170" s="9"/>
       <c r="B170" s="9"/>
       <c r="C170" s="9"/>
+      <c r="E170" s="9"/>
+      <c r="F170" s="9"/>
       <c r="G170" s="9"/>
-      <c r="H170" s="9"/>
-      <c r="I170" s="9"/>
       <c r="J170" s="9"/>
       <c r="K170" s="9"/>
       <c r="L170" s="9"/>
@@ -2450,9 +2452,9 @@
       <c r="A171" s="9"/>
       <c r="B171" s="9"/>
       <c r="C171" s="9"/>
+      <c r="E171" s="9"/>
+      <c r="F171" s="9"/>
       <c r="G171" s="9"/>
-      <c r="H171" s="9"/>
-      <c r="I171" s="9"/>
       <c r="J171" s="9"/>
       <c r="K171" s="9"/>
       <c r="L171" s="9"/>
@@ -2462,9 +2464,9 @@
       <c r="A172" s="9"/>
       <c r="B172" s="9"/>
       <c r="C172" s="9"/>
+      <c r="E172" s="9"/>
+      <c r="F172" s="9"/>
       <c r="G172" s="9"/>
-      <c r="H172" s="9"/>
-      <c r="I172" s="9"/>
       <c r="J172" s="9"/>
       <c r="K172" s="9"/>
       <c r="L172" s="9"/>
@@ -2474,9 +2476,9 @@
       <c r="A173" s="9"/>
       <c r="B173" s="9"/>
       <c r="C173" s="9"/>
+      <c r="E173" s="9"/>
+      <c r="F173" s="9"/>
       <c r="G173" s="9"/>
-      <c r="H173" s="9"/>
-      <c r="I173" s="9"/>
       <c r="J173" s="9"/>
       <c r="K173" s="9"/>
       <c r="L173" s="9"/>
@@ -2486,9 +2488,9 @@
       <c r="A174" s="9"/>
       <c r="B174" s="9"/>
       <c r="C174" s="9"/>
+      <c r="E174" s="9"/>
+      <c r="F174" s="9"/>
       <c r="G174" s="9"/>
-      <c r="H174" s="9"/>
-      <c r="I174" s="9"/>
       <c r="J174" s="9"/>
       <c r="K174" s="9"/>
       <c r="L174" s="9"/>
@@ -2498,9 +2500,9 @@
       <c r="A175" s="9"/>
       <c r="B175" s="9"/>
       <c r="C175" s="9"/>
+      <c r="E175" s="9"/>
+      <c r="F175" s="9"/>
       <c r="G175" s="9"/>
-      <c r="H175" s="9"/>
-      <c r="I175" s="9"/>
       <c r="J175" s="9"/>
       <c r="K175" s="9"/>
       <c r="L175" s="9"/>
@@ -2510,9 +2512,9 @@
       <c r="A176" s="9"/>
       <c r="B176" s="9"/>
       <c r="C176" s="9"/>
+      <c r="E176" s="9"/>
+      <c r="F176" s="9"/>
       <c r="G176" s="9"/>
-      <c r="H176" s="9"/>
-      <c r="I176" s="9"/>
       <c r="J176" s="9"/>
       <c r="K176" s="9"/>
       <c r="L176" s="9"/>
@@ -2522,9 +2524,9 @@
       <c r="A177" s="9"/>
       <c r="B177" s="9"/>
       <c r="C177" s="9"/>
+      <c r="E177" s="9"/>
+      <c r="F177" s="9"/>
       <c r="G177" s="9"/>
-      <c r="H177" s="9"/>
-      <c r="I177" s="9"/>
       <c r="J177" s="9"/>
       <c r="K177" s="9"/>
       <c r="L177" s="9"/>
@@ -2534,9 +2536,9 @@
       <c r="A178" s="9"/>
       <c r="B178" s="9"/>
       <c r="C178" s="9"/>
+      <c r="E178" s="9"/>
+      <c r="F178" s="9"/>
       <c r="G178" s="9"/>
-      <c r="H178" s="9"/>
-      <c r="I178" s="9"/>
       <c r="J178" s="9"/>
       <c r="K178" s="9"/>
       <c r="L178" s="9"/>
@@ -2546,9 +2548,9 @@
       <c r="A179" s="9"/>
       <c r="B179" s="9"/>
       <c r="C179" s="9"/>
+      <c r="E179" s="9"/>
+      <c r="F179" s="9"/>
       <c r="G179" s="9"/>
-      <c r="H179" s="9"/>
-      <c r="I179" s="9"/>
       <c r="J179" s="9"/>
       <c r="K179" s="9"/>
       <c r="L179" s="9"/>
@@ -2558,9 +2560,9 @@
       <c r="A180" s="9"/>
       <c r="B180" s="9"/>
       <c r="C180" s="9"/>
+      <c r="E180" s="9"/>
+      <c r="F180" s="9"/>
       <c r="G180" s="9"/>
-      <c r="H180" s="9"/>
-      <c r="I180" s="9"/>
       <c r="J180" s="9"/>
       <c r="K180" s="9"/>
       <c r="L180" s="9"/>
@@ -2570,9 +2572,9 @@
       <c r="A181" s="9"/>
       <c r="B181" s="9"/>
       <c r="C181" s="9"/>
+      <c r="E181" s="9"/>
+      <c r="F181" s="9"/>
       <c r="G181" s="9"/>
-      <c r="H181" s="9"/>
-      <c r="I181" s="9"/>
       <c r="J181" s="9"/>
       <c r="K181" s="9"/>
       <c r="L181" s="9"/>
@@ -2582,9 +2584,9 @@
       <c r="A182" s="9"/>
       <c r="B182" s="9"/>
       <c r="C182" s="9"/>
+      <c r="E182" s="9"/>
+      <c r="F182" s="9"/>
       <c r="G182" s="9"/>
-      <c r="H182" s="9"/>
-      <c r="I182" s="9"/>
       <c r="J182" s="9"/>
       <c r="K182" s="9"/>
       <c r="L182" s="9"/>
@@ -2594,9 +2596,9 @@
       <c r="A183" s="9"/>
       <c r="B183" s="9"/>
       <c r="C183" s="9"/>
+      <c r="E183" s="9"/>
+      <c r="F183" s="9"/>
       <c r="G183" s="9"/>
-      <c r="H183" s="9"/>
-      <c r="I183" s="9"/>
       <c r="J183" s="9"/>
       <c r="K183" s="9"/>
       <c r="L183" s="9"/>
@@ -2606,9 +2608,9 @@
       <c r="A184" s="9"/>
       <c r="B184" s="9"/>
       <c r="C184" s="9"/>
+      <c r="E184" s="9"/>
+      <c r="F184" s="9"/>
       <c r="G184" s="9"/>
-      <c r="H184" s="9"/>
-      <c r="I184" s="9"/>
       <c r="J184" s="9"/>
       <c r="K184" s="9"/>
       <c r="L184" s="9"/>
@@ -2618,9 +2620,9 @@
       <c r="A185" s="9"/>
       <c r="B185" s="9"/>
       <c r="C185" s="9"/>
+      <c r="E185" s="9"/>
+      <c r="F185" s="9"/>
       <c r="G185" s="9"/>
-      <c r="H185" s="9"/>
-      <c r="I185" s="9"/>
       <c r="J185" s="9"/>
       <c r="K185" s="9"/>
       <c r="L185" s="9"/>
@@ -2630,9 +2632,9 @@
       <c r="A186" s="9"/>
       <c r="B186" s="9"/>
       <c r="C186" s="9"/>
+      <c r="E186" s="9"/>
+      <c r="F186" s="9"/>
       <c r="G186" s="9"/>
-      <c r="H186" s="9"/>
-      <c r="I186" s="9"/>
       <c r="J186" s="9"/>
       <c r="K186" s="9"/>
       <c r="L186" s="9"/>
@@ -2642,9 +2644,9 @@
       <c r="A187" s="9"/>
       <c r="B187" s="9"/>
       <c r="C187" s="9"/>
+      <c r="E187" s="9"/>
+      <c r="F187" s="9"/>
       <c r="G187" s="9"/>
-      <c r="H187" s="9"/>
-      <c r="I187" s="9"/>
       <c r="J187" s="9"/>
       <c r="K187" s="9"/>
       <c r="L187" s="9"/>
@@ -2654,9 +2656,9 @@
       <c r="A188" s="9"/>
       <c r="B188" s="9"/>
       <c r="C188" s="9"/>
+      <c r="E188" s="9"/>
+      <c r="F188" s="9"/>
       <c r="G188" s="9"/>
-      <c r="H188" s="9"/>
-      <c r="I188" s="9"/>
       <c r="J188" s="9"/>
       <c r="K188" s="9"/>
       <c r="L188" s="9"/>
@@ -2666,9 +2668,9 @@
       <c r="A189" s="9"/>
       <c r="B189" s="9"/>
       <c r="C189" s="9"/>
+      <c r="E189" s="9"/>
+      <c r="F189" s="9"/>
       <c r="G189" s="9"/>
-      <c r="H189" s="9"/>
-      <c r="I189" s="9"/>
       <c r="J189" s="9"/>
       <c r="K189" s="9"/>
       <c r="L189" s="9"/>
@@ -2678,9 +2680,9 @@
       <c r="A190" s="9"/>
       <c r="B190" s="9"/>
       <c r="C190" s="9"/>
+      <c r="E190" s="9"/>
+      <c r="F190" s="9"/>
       <c r="G190" s="9"/>
-      <c r="H190" s="9"/>
-      <c r="I190" s="9"/>
       <c r="J190" s="9"/>
       <c r="K190" s="9"/>
       <c r="L190" s="9"/>
@@ -2690,9 +2692,9 @@
       <c r="A191" s="9"/>
       <c r="B191" s="9"/>
       <c r="C191" s="9"/>
+      <c r="E191" s="9"/>
+      <c r="F191" s="9"/>
       <c r="G191" s="9"/>
-      <c r="H191" s="9"/>
-      <c r="I191" s="9"/>
       <c r="J191" s="9"/>
       <c r="K191" s="9"/>
       <c r="L191" s="9"/>
@@ -2702,9 +2704,9 @@
       <c r="A192" s="9"/>
       <c r="B192" s="9"/>
       <c r="C192" s="9"/>
+      <c r="E192" s="9"/>
+      <c r="F192" s="9"/>
       <c r="G192" s="9"/>
-      <c r="H192" s="9"/>
-      <c r="I192" s="9"/>
       <c r="J192" s="9"/>
       <c r="K192" s="9"/>
       <c r="L192" s="9"/>
@@ -2714,9 +2716,9 @@
       <c r="A193" s="9"/>
       <c r="B193" s="9"/>
       <c r="C193" s="9"/>
+      <c r="E193" s="9"/>
+      <c r="F193" s="9"/>
       <c r="G193" s="9"/>
-      <c r="H193" s="9"/>
-      <c r="I193" s="9"/>
       <c r="J193" s="9"/>
       <c r="K193" s="9"/>
       <c r="L193" s="9"/>
@@ -2726,9 +2728,9 @@
       <c r="A194" s="9"/>
       <c r="B194" s="9"/>
       <c r="C194" s="9"/>
+      <c r="E194" s="9"/>
+      <c r="F194" s="9"/>
       <c r="G194" s="9"/>
-      <c r="H194" s="9"/>
-      <c r="I194" s="9"/>
       <c r="J194" s="9"/>
       <c r="K194" s="9"/>
       <c r="L194" s="9"/>
@@ -2738,9 +2740,9 @@
       <c r="A195" s="9"/>
       <c r="B195" s="9"/>
       <c r="C195" s="9"/>
+      <c r="E195" s="9"/>
+      <c r="F195" s="9"/>
       <c r="G195" s="9"/>
-      <c r="H195" s="9"/>
-      <c r="I195" s="9"/>
       <c r="J195" s="9"/>
       <c r="K195" s="9"/>
       <c r="L195" s="9"/>
@@ -2750,9 +2752,9 @@
       <c r="A196" s="9"/>
       <c r="B196" s="9"/>
       <c r="C196" s="9"/>
+      <c r="E196" s="9"/>
+      <c r="F196" s="9"/>
       <c r="G196" s="9"/>
-      <c r="H196" s="9"/>
-      <c r="I196" s="9"/>
       <c r="J196" s="9"/>
       <c r="K196" s="9"/>
       <c r="L196" s="9"/>
@@ -2762,9 +2764,9 @@
       <c r="A197" s="9"/>
       <c r="B197" s="9"/>
       <c r="C197" s="9"/>
+      <c r="E197" s="9"/>
+      <c r="F197" s="9"/>
       <c r="G197" s="9"/>
-      <c r="H197" s="9"/>
-      <c r="I197" s="9"/>
       <c r="J197" s="9"/>
       <c r="K197" s="9"/>
       <c r="L197" s="9"/>
@@ -2774,9 +2776,9 @@
       <c r="A198" s="9"/>
       <c r="B198" s="9"/>
       <c r="C198" s="9"/>
+      <c r="E198" s="9"/>
+      <c r="F198" s="9"/>
       <c r="G198" s="9"/>
-      <c r="H198" s="9"/>
-      <c r="I198" s="9"/>
       <c r="J198" s="9"/>
       <c r="K198" s="9"/>
       <c r="L198" s="9"/>
@@ -2786,9 +2788,9 @@
       <c r="A199" s="9"/>
       <c r="B199" s="9"/>
       <c r="C199" s="9"/>
+      <c r="E199" s="9"/>
+      <c r="F199" s="9"/>
       <c r="G199" s="9"/>
-      <c r="H199" s="9"/>
-      <c r="I199" s="9"/>
       <c r="J199" s="9"/>
       <c r="K199" s="9"/>
       <c r="L199" s="9"/>
@@ -2798,9 +2800,9 @@
       <c r="A200" s="9"/>
       <c r="B200" s="9"/>
       <c r="C200" s="9"/>
+      <c r="E200" s="9"/>
+      <c r="F200" s="9"/>
       <c r="G200" s="9"/>
-      <c r="H200" s="9"/>
-      <c r="I200" s="9"/>
       <c r="J200" s="9"/>
       <c r="K200" s="9"/>
       <c r="L200" s="9"/>
@@ -2810,9 +2812,9 @@
       <c r="A201" s="9"/>
       <c r="B201" s="9"/>
       <c r="C201" s="9"/>
+      <c r="E201" s="9"/>
+      <c r="F201" s="9"/>
       <c r="G201" s="9"/>
-      <c r="H201" s="9"/>
-      <c r="I201" s="9"/>
       <c r="J201" s="9"/>
       <c r="K201" s="9"/>
       <c r="L201" s="9"/>
@@ -2822,9 +2824,9 @@
       <c r="A202" s="9"/>
       <c r="B202" s="9"/>
       <c r="C202" s="9"/>
+      <c r="E202" s="9"/>
+      <c r="F202" s="9"/>
       <c r="G202" s="9"/>
-      <c r="H202" s="9"/>
-      <c r="I202" s="9"/>
       <c r="J202" s="9"/>
       <c r="K202" s="9"/>
       <c r="L202" s="9"/>
@@ -2834,9 +2836,9 @@
       <c r="A203" s="9"/>
       <c r="B203" s="9"/>
       <c r="C203" s="9"/>
+      <c r="E203" s="9"/>
+      <c r="F203" s="9"/>
       <c r="G203" s="9"/>
-      <c r="H203" s="9"/>
-      <c r="I203" s="9"/>
       <c r="J203" s="9"/>
       <c r="K203" s="9"/>
       <c r="L203" s="9"/>
@@ -2846,9 +2848,9 @@
       <c r="A204" s="9"/>
       <c r="B204" s="9"/>
       <c r="C204" s="9"/>
+      <c r="E204" s="9"/>
+      <c r="F204" s="9"/>
       <c r="G204" s="9"/>
-      <c r="H204" s="9"/>
-      <c r="I204" s="9"/>
       <c r="J204" s="9"/>
       <c r="K204" s="9"/>
       <c r="L204" s="9"/>
@@ -2858,9 +2860,9 @@
       <c r="A205" s="9"/>
       <c r="B205" s="9"/>
       <c r="C205" s="9"/>
+      <c r="E205" s="9"/>
+      <c r="F205" s="9"/>
       <c r="G205" s="9"/>
-      <c r="H205" s="9"/>
-      <c r="I205" s="9"/>
       <c r="J205" s="9"/>
       <c r="K205" s="9"/>
       <c r="L205" s="9"/>
@@ -2870,9 +2872,9 @@
       <c r="A206" s="9"/>
       <c r="B206" s="9"/>
       <c r="C206" s="9"/>
+      <c r="E206" s="9"/>
+      <c r="F206" s="9"/>
       <c r="G206" s="9"/>
-      <c r="H206" s="9"/>
-      <c r="I206" s="9"/>
       <c r="J206" s="9"/>
       <c r="K206" s="9"/>
       <c r="L206" s="9"/>
@@ -2882,9 +2884,9 @@
       <c r="A207" s="9"/>
       <c r="B207" s="9"/>
       <c r="C207" s="9"/>
+      <c r="E207" s="9"/>
+      <c r="F207" s="9"/>
       <c r="G207" s="9"/>
-      <c r="H207" s="9"/>
-      <c r="I207" s="9"/>
       <c r="J207" s="9"/>
       <c r="K207" s="9"/>
       <c r="L207" s="9"/>
@@ -2894,9 +2896,9 @@
       <c r="A208" s="9"/>
       <c r="B208" s="9"/>
       <c r="C208" s="9"/>
+      <c r="E208" s="9"/>
+      <c r="F208" s="9"/>
       <c r="G208" s="9"/>
-      <c r="H208" s="9"/>
-      <c r="I208" s="9"/>
       <c r="J208" s="9"/>
       <c r="K208" s="9"/>
       <c r="L208" s="9"/>
@@ -2906,9 +2908,9 @@
       <c r="A209" s="9"/>
       <c r="B209" s="9"/>
       <c r="C209" s="9"/>
+      <c r="E209" s="9"/>
+      <c r="F209" s="9"/>
       <c r="G209" s="9"/>
-      <c r="H209" s="9"/>
-      <c r="I209" s="9"/>
       <c r="J209" s="9"/>
       <c r="K209" s="9"/>
       <c r="L209" s="9"/>
@@ -2918,9 +2920,9 @@
       <c r="A210" s="9"/>
       <c r="B210" s="9"/>
       <c r="C210" s="9"/>
+      <c r="E210" s="9"/>
+      <c r="F210" s="9"/>
       <c r="G210" s="9"/>
-      <c r="H210" s="9"/>
-      <c r="I210" s="9"/>
       <c r="J210" s="9"/>
       <c r="K210" s="9"/>
       <c r="L210" s="9"/>
@@ -2930,9 +2932,9 @@
       <c r="A211" s="9"/>
       <c r="B211" s="9"/>
       <c r="C211" s="9"/>
+      <c r="E211" s="9"/>
+      <c r="F211" s="9"/>
       <c r="G211" s="9"/>
-      <c r="H211" s="9"/>
-      <c r="I211" s="9"/>
       <c r="J211" s="9"/>
       <c r="K211" s="9"/>
       <c r="L211" s="9"/>
@@ -2942,9 +2944,9 @@
       <c r="A212" s="9"/>
       <c r="B212" s="9"/>
       <c r="C212" s="9"/>
+      <c r="E212" s="9"/>
+      <c r="F212" s="9"/>
       <c r="G212" s="9"/>
-      <c r="H212" s="9"/>
-      <c r="I212" s="9"/>
       <c r="J212" s="9"/>
       <c r="K212" s="9"/>
       <c r="L212" s="9"/>
@@ -2954,9 +2956,9 @@
       <c r="A213" s="9"/>
       <c r="B213" s="9"/>
       <c r="C213" s="9"/>
+      <c r="E213" s="9"/>
+      <c r="F213" s="9"/>
       <c r="G213" s="9"/>
-      <c r="H213" s="9"/>
-      <c r="I213" s="9"/>
       <c r="J213" s="9"/>
       <c r="K213" s="9"/>
       <c r="L213" s="9"/>
@@ -2966,9 +2968,9 @@
       <c r="A214" s="9"/>
       <c r="B214" s="9"/>
       <c r="C214" s="9"/>
+      <c r="E214" s="9"/>
+      <c r="F214" s="9"/>
       <c r="G214" s="9"/>
-      <c r="H214" s="9"/>
-      <c r="I214" s="9"/>
       <c r="J214" s="9"/>
       <c r="K214" s="9"/>
       <c r="L214" s="9"/>
@@ -2978,9 +2980,9 @@
       <c r="A215" s="9"/>
       <c r="B215" s="9"/>
       <c r="C215" s="9"/>
+      <c r="E215" s="9"/>
+      <c r="F215" s="9"/>
       <c r="G215" s="9"/>
-      <c r="H215" s="9"/>
-      <c r="I215" s="9"/>
       <c r="J215" s="9"/>
       <c r="K215" s="9"/>
       <c r="L215" s="9"/>
@@ -2990,9 +2992,9 @@
       <c r="A216" s="9"/>
       <c r="B216" s="9"/>
       <c r="C216" s="9"/>
+      <c r="E216" s="9"/>
+      <c r="F216" s="9"/>
       <c r="G216" s="9"/>
-      <c r="H216" s="9"/>
-      <c r="I216" s="9"/>
       <c r="J216" s="9"/>
       <c r="K216" s="9"/>
       <c r="L216" s="9"/>
@@ -3002,9 +3004,9 @@
       <c r="A217" s="9"/>
       <c r="B217" s="9"/>
       <c r="C217" s="9"/>
+      <c r="E217" s="9"/>
+      <c r="F217" s="9"/>
       <c r="G217" s="9"/>
-      <c r="H217" s="9"/>
-      <c r="I217" s="9"/>
       <c r="J217" s="9"/>
       <c r="K217" s="9"/>
       <c r="L217" s="9"/>
@@ -3014,9 +3016,9 @@
       <c r="A218" s="9"/>
       <c r="B218" s="9"/>
       <c r="C218" s="9"/>
+      <c r="E218" s="9"/>
+      <c r="F218" s="9"/>
       <c r="G218" s="9"/>
-      <c r="H218" s="9"/>
-      <c r="I218" s="9"/>
       <c r="J218" s="9"/>
       <c r="K218" s="9"/>
       <c r="L218" s="9"/>
@@ -3026,9 +3028,9 @@
       <c r="A219" s="9"/>
       <c r="B219" s="9"/>
       <c r="C219" s="9"/>
+      <c r="E219" s="9"/>
+      <c r="F219" s="9"/>
       <c r="G219" s="9"/>
-      <c r="H219" s="9"/>
-      <c r="I219" s="9"/>
       <c r="J219" s="9"/>
       <c r="K219" s="9"/>
       <c r="L219" s="9"/>
@@ -3038,9 +3040,9 @@
       <c r="A220" s="9"/>
       <c r="B220" s="9"/>
       <c r="C220" s="9"/>
+      <c r="E220" s="9"/>
+      <c r="F220" s="9"/>
       <c r="G220" s="9"/>
-      <c r="H220" s="9"/>
-      <c r="I220" s="9"/>
       <c r="J220" s="9"/>
       <c r="K220" s="9"/>
       <c r="L220" s="9"/>
@@ -3050,9 +3052,9 @@
       <c r="A221" s="9"/>
       <c r="B221" s="9"/>
       <c r="C221" s="9"/>
+      <c r="E221" s="9"/>
+      <c r="F221" s="9"/>
       <c r="G221" s="9"/>
-      <c r="H221" s="9"/>
-      <c r="I221" s="9"/>
       <c r="J221" s="9"/>
       <c r="K221" s="9"/>
       <c r="L221" s="9"/>
@@ -3062,9 +3064,9 @@
       <c r="A222" s="9"/>
       <c r="B222" s="9"/>
       <c r="C222" s="9"/>
+      <c r="E222" s="9"/>
+      <c r="F222" s="9"/>
       <c r="G222" s="9"/>
-      <c r="H222" s="9"/>
-      <c r="I222" s="9"/>
       <c r="J222" s="9"/>
       <c r="K222" s="9"/>
       <c r="L222" s="9"/>
@@ -3074,9 +3076,9 @@
       <c r="A223" s="9"/>
       <c r="B223" s="9"/>
       <c r="C223" s="9"/>
+      <c r="E223" s="9"/>
+      <c r="F223" s="9"/>
       <c r="G223" s="9"/>
-      <c r="H223" s="9"/>
-      <c r="I223" s="9"/>
       <c r="J223" s="9"/>
       <c r="K223" s="9"/>
       <c r="L223" s="9"/>
@@ -3086,9 +3088,9 @@
       <c r="A224" s="9"/>
       <c r="B224" s="9"/>
       <c r="C224" s="9"/>
+      <c r="E224" s="9"/>
+      <c r="F224" s="9"/>
       <c r="G224" s="9"/>
-      <c r="H224" s="9"/>
-      <c r="I224" s="9"/>
       <c r="J224" s="9"/>
       <c r="K224" s="9"/>
       <c r="L224" s="9"/>
@@ -3098,9 +3100,9 @@
       <c r="A225" s="9"/>
       <c r="B225" s="9"/>
       <c r="C225" s="9"/>
+      <c r="E225" s="9"/>
+      <c r="F225" s="9"/>
       <c r="G225" s="9"/>
-      <c r="H225" s="9"/>
-      <c r="I225" s="9"/>
       <c r="J225" s="9"/>
       <c r="K225" s="9"/>
       <c r="L225" s="9"/>
@@ -3110,9 +3112,9 @@
       <c r="A226" s="9"/>
       <c r="B226" s="9"/>
       <c r="C226" s="9"/>
+      <c r="E226" s="9"/>
+      <c r="F226" s="9"/>
       <c r="G226" s="9"/>
-      <c r="H226" s="9"/>
-      <c r="I226" s="9"/>
       <c r="J226" s="9"/>
       <c r="K226" s="9"/>
       <c r="L226" s="9"/>
@@ -3122,9 +3124,9 @@
       <c r="A227" s="9"/>
       <c r="B227" s="9"/>
       <c r="C227" s="9"/>
+      <c r="E227" s="9"/>
+      <c r="F227" s="9"/>
       <c r="G227" s="9"/>
-      <c r="H227" s="9"/>
-      <c r="I227" s="9"/>
       <c r="J227" s="9"/>
       <c r="K227" s="9"/>
       <c r="L227" s="9"/>
@@ -3134,9 +3136,9 @@
       <c r="A228" s="9"/>
       <c r="B228" s="9"/>
       <c r="C228" s="9"/>
+      <c r="E228" s="9"/>
+      <c r="F228" s="9"/>
       <c r="G228" s="9"/>
-      <c r="H228" s="9"/>
-      <c r="I228" s="9"/>
       <c r="J228" s="9"/>
       <c r="K228" s="9"/>
       <c r="L228" s="9"/>
@@ -3146,9 +3148,9 @@
       <c r="A229" s="9"/>
       <c r="B229" s="9"/>
       <c r="C229" s="9"/>
+      <c r="E229" s="9"/>
+      <c r="F229" s="9"/>
       <c r="G229" s="9"/>
-      <c r="H229" s="9"/>
-      <c r="I229" s="9"/>
       <c r="J229" s="9"/>
       <c r="K229" s="9"/>
       <c r="L229" s="9"/>
@@ -3158,9 +3160,9 @@
       <c r="A230" s="9"/>
       <c r="B230" s="9"/>
       <c r="C230" s="9"/>
+      <c r="E230" s="9"/>
+      <c r="F230" s="9"/>
       <c r="G230" s="9"/>
-      <c r="H230" s="9"/>
-      <c r="I230" s="9"/>
       <c r="J230" s="9"/>
       <c r="K230" s="9"/>
       <c r="L230" s="9"/>
@@ -3170,9 +3172,9 @@
       <c r="A231" s="9"/>
       <c r="B231" s="9"/>
       <c r="C231" s="9"/>
+      <c r="E231" s="9"/>
+      <c r="F231" s="9"/>
       <c r="G231" s="9"/>
-      <c r="H231" s="9"/>
-      <c r="I231" s="9"/>
       <c r="J231" s="9"/>
       <c r="K231" s="9"/>
       <c r="L231" s="9"/>
@@ -3182,9 +3184,9 @@
       <c r="A232" s="9"/>
       <c r="B232" s="9"/>
       <c r="C232" s="9"/>
+      <c r="E232" s="9"/>
+      <c r="F232" s="9"/>
       <c r="G232" s="9"/>
-      <c r="H232" s="9"/>
-      <c r="I232" s="9"/>
       <c r="J232" s="9"/>
       <c r="K232" s="9"/>
       <c r="L232" s="9"/>
@@ -3194,9 +3196,9 @@
       <c r="A233" s="9"/>
       <c r="B233" s="9"/>
       <c r="C233" s="9"/>
+      <c r="E233" s="9"/>
+      <c r="F233" s="9"/>
       <c r="G233" s="9"/>
-      <c r="H233" s="9"/>
-      <c r="I233" s="9"/>
       <c r="J233" s="9"/>
       <c r="K233" s="9"/>
       <c r="L233" s="9"/>
@@ -3206,9 +3208,9 @@
       <c r="A234" s="9"/>
       <c r="B234" s="9"/>
       <c r="C234" s="9"/>
+      <c r="E234" s="9"/>
+      <c r="F234" s="9"/>
       <c r="G234" s="9"/>
-      <c r="H234" s="9"/>
-      <c r="I234" s="9"/>
       <c r="J234" s="9"/>
       <c r="K234" s="9"/>
       <c r="L234" s="9"/>
@@ -3218,9 +3220,9 @@
       <c r="A235" s="9"/>
       <c r="B235" s="9"/>
       <c r="C235" s="9"/>
+      <c r="E235" s="9"/>
+      <c r="F235" s="9"/>
       <c r="G235" s="9"/>
-      <c r="H235" s="9"/>
-      <c r="I235" s="9"/>
       <c r="J235" s="9"/>
       <c r="K235" s="9"/>
       <c r="L235" s="9"/>
@@ -3230,9 +3232,9 @@
       <c r="A236" s="9"/>
       <c r="B236" s="9"/>
       <c r="C236" s="9"/>
+      <c r="E236" s="9"/>
+      <c r="F236" s="9"/>
       <c r="G236" s="9"/>
-      <c r="H236" s="9"/>
-      <c r="I236" s="9"/>
       <c r="J236" s="9"/>
       <c r="K236" s="9"/>
       <c r="L236" s="9"/>
@@ -3242,9 +3244,9 @@
       <c r="A237" s="9"/>
       <c r="B237" s="9"/>
       <c r="C237" s="9"/>
+      <c r="E237" s="9"/>
+      <c r="F237" s="9"/>
       <c r="G237" s="9"/>
-      <c r="H237" s="9"/>
-      <c r="I237" s="9"/>
       <c r="J237" s="9"/>
       <c r="K237" s="9"/>
       <c r="L237" s="9"/>
@@ -3254,9 +3256,9 @@
       <c r="A238" s="9"/>
       <c r="B238" s="9"/>
       <c r="C238" s="9"/>
+      <c r="E238" s="9"/>
+      <c r="F238" s="9"/>
       <c r="G238" s="9"/>
-      <c r="H238" s="9"/>
-      <c r="I238" s="9"/>
       <c r="J238" s="9"/>
       <c r="K238" s="9"/>
       <c r="L238" s="9"/>
@@ -3266,9 +3268,9 @@
       <c r="A239" s="9"/>
       <c r="B239" s="9"/>
       <c r="C239" s="9"/>
+      <c r="E239" s="9"/>
+      <c r="F239" s="9"/>
       <c r="G239" s="9"/>
-      <c r="H239" s="9"/>
-      <c r="I239" s="9"/>
       <c r="J239" s="9"/>
       <c r="K239" s="9"/>
       <c r="L239" s="9"/>
@@ -3278,9 +3280,9 @@
       <c r="A240" s="9"/>
       <c r="B240" s="9"/>
       <c r="C240" s="9"/>
+      <c r="E240" s="9"/>
+      <c r="F240" s="9"/>
       <c r="G240" s="9"/>
-      <c r="H240" s="9"/>
-      <c r="I240" s="9"/>
       <c r="J240" s="9"/>
       <c r="K240" s="9"/>
       <c r="L240" s="9"/>
@@ -3290,9 +3292,9 @@
       <c r="A241" s="9"/>
       <c r="B241" s="9"/>
       <c r="C241" s="9"/>
+      <c r="E241" s="9"/>
+      <c r="F241" s="9"/>
       <c r="G241" s="9"/>
-      <c r="H241" s="9"/>
-      <c r="I241" s="9"/>
       <c r="J241" s="9"/>
       <c r="K241" s="9"/>
       <c r="L241" s="9"/>
@@ -3302,9 +3304,9 @@
       <c r="A242" s="9"/>
       <c r="B242" s="9"/>
       <c r="C242" s="9"/>
+      <c r="E242" s="9"/>
+      <c r="F242" s="9"/>
       <c r="G242" s="9"/>
-      <c r="H242" s="9"/>
-      <c r="I242" s="9"/>
       <c r="J242" s="9"/>
       <c r="K242" s="9"/>
       <c r="L242" s="9"/>
@@ -3314,9 +3316,9 @@
       <c r="A243" s="9"/>
       <c r="B243" s="9"/>
       <c r="C243" s="9"/>
+      <c r="E243" s="9"/>
+      <c r="F243" s="9"/>
       <c r="G243" s="9"/>
-      <c r="H243" s="9"/>
-      <c r="I243" s="9"/>
       <c r="J243" s="9"/>
       <c r="K243" s="9"/>
       <c r="L243" s="9"/>
@@ -3326,9 +3328,9 @@
       <c r="A244" s="9"/>
       <c r="B244" s="9"/>
       <c r="C244" s="9"/>
+      <c r="E244" s="9"/>
+      <c r="F244" s="9"/>
       <c r="G244" s="9"/>
-      <c r="H244" s="9"/>
-      <c r="I244" s="9"/>
       <c r="J244" s="9"/>
       <c r="K244" s="9"/>
       <c r="L244" s="9"/>
@@ -3338,9 +3340,9 @@
       <c r="A245" s="9"/>
       <c r="B245" s="9"/>
       <c r="C245" s="9"/>
+      <c r="E245" s="9"/>
+      <c r="F245" s="9"/>
       <c r="G245" s="9"/>
-      <c r="H245" s="9"/>
-      <c r="I245" s="9"/>
       <c r="J245" s="9"/>
       <c r="K245" s="9"/>
       <c r="L245" s="9"/>
@@ -3350,9 +3352,9 @@
       <c r="A246" s="9"/>
       <c r="B246" s="9"/>
       <c r="C246" s="9"/>
+      <c r="E246" s="9"/>
+      <c r="F246" s="9"/>
       <c r="G246" s="9"/>
-      <c r="H246" s="9"/>
-      <c r="I246" s="9"/>
       <c r="J246" s="9"/>
       <c r="K246" s="9"/>
       <c r="L246" s="9"/>
@@ -3362,9 +3364,9 @@
       <c r="A247" s="9"/>
       <c r="B247" s="9"/>
       <c r="C247" s="9"/>
+      <c r="E247" s="9"/>
+      <c r="F247" s="9"/>
       <c r="G247" s="9"/>
-      <c r="H247" s="9"/>
-      <c r="I247" s="9"/>
       <c r="J247" s="9"/>
       <c r="K247" s="9"/>
       <c r="L247" s="9"/>
@@ -3374,9 +3376,9 @@
       <c r="A248" s="9"/>
       <c r="B248" s="9"/>
       <c r="C248" s="9"/>
+      <c r="E248" s="9"/>
+      <c r="F248" s="9"/>
       <c r="G248" s="9"/>
-      <c r="H248" s="9"/>
-      <c r="I248" s="9"/>
       <c r="J248" s="9"/>
       <c r="K248" s="9"/>
       <c r="L248" s="9"/>
@@ -3386,9 +3388,9 @@
       <c r="A249" s="9"/>
       <c r="B249" s="9"/>
       <c r="C249" s="9"/>
+      <c r="E249" s="9"/>
+      <c r="F249" s="9"/>
       <c r="G249" s="9"/>
-      <c r="H249" s="9"/>
-      <c r="I249" s="9"/>
       <c r="J249" s="9"/>
       <c r="K249" s="9"/>
       <c r="L249" s="9"/>
@@ -3398,9 +3400,9 @@
       <c r="A250" s="9"/>
       <c r="B250" s="9"/>
       <c r="C250" s="9"/>
+      <c r="E250" s="9"/>
+      <c r="F250" s="9"/>
       <c r="G250" s="9"/>
-      <c r="H250" s="9"/>
-      <c r="I250" s="9"/>
       <c r="J250" s="9"/>
       <c r="K250" s="9"/>
       <c r="L250" s="9"/>
@@ -3410,9 +3412,9 @@
       <c r="A251" s="9"/>
       <c r="B251" s="9"/>
       <c r="C251" s="9"/>
+      <c r="E251" s="9"/>
+      <c r="F251" s="9"/>
       <c r="G251" s="9"/>
-      <c r="H251" s="9"/>
-      <c r="I251" s="9"/>
       <c r="J251" s="9"/>
       <c r="K251" s="9"/>
       <c r="L251" s="9"/>
@@ -3422,9 +3424,9 @@
       <c r="A252" s="9"/>
       <c r="B252" s="9"/>
       <c r="C252" s="9"/>
+      <c r="E252" s="9"/>
+      <c r="F252" s="9"/>
       <c r="G252" s="9"/>
-      <c r="H252" s="9"/>
-      <c r="I252" s="9"/>
       <c r="J252" s="9"/>
       <c r="K252" s="9"/>
       <c r="L252" s="9"/>
@@ -3434,9 +3436,9 @@
       <c r="A253" s="9"/>
       <c r="B253" s="9"/>
       <c r="C253" s="9"/>
+      <c r="E253" s="9"/>
+      <c r="F253" s="9"/>
       <c r="G253" s="9"/>
-      <c r="H253" s="9"/>
-      <c r="I253" s="9"/>
       <c r="J253" s="9"/>
       <c r="K253" s="9"/>
       <c r="L253" s="9"/>
@@ -3446,9 +3448,9 @@
       <c r="A254" s="9"/>
       <c r="B254" s="9"/>
       <c r="C254" s="9"/>
+      <c r="E254" s="9"/>
+      <c r="F254" s="9"/>
       <c r="G254" s="9"/>
-      <c r="H254" s="9"/>
-      <c r="I254" s="9"/>
       <c r="J254" s="9"/>
       <c r="K254" s="9"/>
       <c r="L254" s="9"/>
@@ -3458,9 +3460,9 @@
       <c r="A255" s="9"/>
       <c r="B255" s="9"/>
       <c r="C255" s="9"/>
+      <c r="E255" s="9"/>
+      <c r="F255" s="9"/>
       <c r="G255" s="9"/>
-      <c r="H255" s="9"/>
-      <c r="I255" s="9"/>
       <c r="J255" s="9"/>
       <c r="K255" s="9"/>
       <c r="L255" s="9"/>
@@ -3470,9 +3472,9 @@
       <c r="A256" s="9"/>
       <c r="B256" s="9"/>
       <c r="C256" s="9"/>
+      <c r="E256" s="9"/>
+      <c r="F256" s="9"/>
       <c r="G256" s="9"/>
-      <c r="H256" s="9"/>
-      <c r="I256" s="9"/>
       <c r="J256" s="9"/>
       <c r="K256" s="9"/>
       <c r="L256" s="9"/>
@@ -3482,9 +3484,9 @@
       <c r="A257" s="9"/>
       <c r="B257" s="9"/>
       <c r="C257" s="9"/>
+      <c r="E257" s="9"/>
+      <c r="F257" s="9"/>
       <c r="G257" s="9"/>
-      <c r="H257" s="9"/>
-      <c r="I257" s="9"/>
       <c r="J257" s="9"/>
       <c r="K257" s="9"/>
       <c r="L257" s="9"/>
@@ -3494,9 +3496,9 @@
       <c r="A258" s="9"/>
       <c r="B258" s="9"/>
       <c r="C258" s="9"/>
+      <c r="E258" s="9"/>
+      <c r="F258" s="9"/>
       <c r="G258" s="9"/>
-      <c r="H258" s="9"/>
-      <c r="I258" s="9"/>
       <c r="J258" s="9"/>
       <c r="K258" s="9"/>
       <c r="L258" s="9"/>
@@ -3506,9 +3508,9 @@
       <c r="A259" s="9"/>
       <c r="B259" s="9"/>
       <c r="C259" s="9"/>
+      <c r="E259" s="9"/>
+      <c r="F259" s="9"/>
       <c r="G259" s="9"/>
-      <c r="H259" s="9"/>
-      <c r="I259" s="9"/>
       <c r="J259" s="9"/>
       <c r="K259" s="9"/>
       <c r="L259" s="9"/>
@@ -3518,9 +3520,9 @@
       <c r="A260" s="9"/>
       <c r="B260" s="9"/>
       <c r="C260" s="9"/>
+      <c r="E260" s="9"/>
+      <c r="F260" s="9"/>
       <c r="G260" s="9"/>
-      <c r="H260" s="9"/>
-      <c r="I260" s="9"/>
       <c r="J260" s="9"/>
       <c r="K260" s="9"/>
       <c r="L260" s="9"/>
@@ -3530,9 +3532,9 @@
       <c r="A261" s="9"/>
       <c r="B261" s="9"/>
       <c r="C261" s="9"/>
+      <c r="E261" s="9"/>
+      <c r="F261" s="9"/>
       <c r="G261" s="9"/>
-      <c r="H261" s="9"/>
-      <c r="I261" s="9"/>
       <c r="J261" s="9"/>
       <c r="K261" s="9"/>
       <c r="L261" s="9"/>
@@ -3542,9 +3544,9 @@
       <c r="A262" s="9"/>
       <c r="B262" s="9"/>
       <c r="C262" s="9"/>
+      <c r="E262" s="9"/>
+      <c r="F262" s="9"/>
       <c r="G262" s="9"/>
-      <c r="H262" s="9"/>
-      <c r="I262" s="9"/>
       <c r="J262" s="9"/>
       <c r="K262" s="9"/>
       <c r="L262" s="9"/>
@@ -3554,9 +3556,9 @@
       <c r="A263" s="9"/>
       <c r="B263" s="9"/>
       <c r="C263" s="9"/>
+      <c r="E263" s="9"/>
+      <c r="F263" s="9"/>
       <c r="G263" s="9"/>
-      <c r="H263" s="9"/>
-      <c r="I263" s="9"/>
       <c r="J263" s="9"/>
       <c r="K263" s="9"/>
       <c r="L263" s="9"/>
@@ -3566,9 +3568,9 @@
       <c r="A264" s="9"/>
       <c r="B264" s="9"/>
       <c r="C264" s="9"/>
+      <c r="E264" s="9"/>
+      <c r="F264" s="9"/>
       <c r="G264" s="9"/>
-      <c r="H264" s="9"/>
-      <c r="I264" s="9"/>
       <c r="J264" s="9"/>
       <c r="K264" s="9"/>
       <c r="L264" s="9"/>
@@ -3578,9 +3580,9 @@
       <c r="A265" s="9"/>
       <c r="B265" s="9"/>
       <c r="C265" s="9"/>
+      <c r="E265" s="9"/>
+      <c r="F265" s="9"/>
       <c r="G265" s="9"/>
-      <c r="H265" s="9"/>
-      <c r="I265" s="9"/>
       <c r="J265" s="9"/>
       <c r="K265" s="9"/>
       <c r="L265" s="9"/>
@@ -3590,9 +3592,9 @@
       <c r="A266" s="9"/>
       <c r="B266" s="9"/>
       <c r="C266" s="9"/>
+      <c r="E266" s="9"/>
+      <c r="F266" s="9"/>
       <c r="G266" s="9"/>
-      <c r="H266" s="9"/>
-      <c r="I266" s="9"/>
       <c r="J266" s="9"/>
       <c r="K266" s="9"/>
       <c r="L266" s="9"/>
@@ -3602,9 +3604,9 @@
       <c r="A267" s="9"/>
       <c r="B267" s="9"/>
       <c r="C267" s="9"/>
+      <c r="E267" s="9"/>
+      <c r="F267" s="9"/>
       <c r="G267" s="9"/>
-      <c r="H267" s="9"/>
-      <c r="I267" s="9"/>
       <c r="J267" s="9"/>
       <c r="K267" s="9"/>
       <c r="L267" s="9"/>
@@ -3614,9 +3616,9 @@
       <c r="A268" s="9"/>
       <c r="B268" s="9"/>
       <c r="C268" s="9"/>
+      <c r="E268" s="9"/>
+      <c r="F268" s="9"/>
       <c r="G268" s="9"/>
-      <c r="H268" s="9"/>
-      <c r="I268" s="9"/>
       <c r="J268" s="9"/>
       <c r="K268" s="9"/>
       <c r="L268" s="9"/>
@@ -3626,9 +3628,9 @@
       <c r="A269" s="9"/>
       <c r="B269" s="9"/>
       <c r="C269" s="9"/>
+      <c r="E269" s="9"/>
+      <c r="F269" s="9"/>
       <c r="G269" s="9"/>
-      <c r="H269" s="9"/>
-      <c r="I269" s="9"/>
       <c r="J269" s="9"/>
       <c r="K269" s="9"/>
       <c r="L269" s="9"/>
@@ -3638,9 +3640,9 @@
       <c r="A270" s="9"/>
       <c r="B270" s="9"/>
       <c r="C270" s="9"/>
+      <c r="E270" s="9"/>
+      <c r="F270" s="9"/>
       <c r="G270" s="9"/>
-      <c r="H270" s="9"/>
-      <c r="I270" s="9"/>
       <c r="J270" s="9"/>
       <c r="K270" s="9"/>
       <c r="L270" s="9"/>
@@ -3650,9 +3652,9 @@
       <c r="A271" s="9"/>
       <c r="B271" s="9"/>
       <c r="C271" s="9"/>
+      <c r="E271" s="9"/>
+      <c r="F271" s="9"/>
       <c r="G271" s="9"/>
-      <c r="H271" s="9"/>
-      <c r="I271" s="9"/>
       <c r="J271" s="9"/>
       <c r="K271" s="9"/>
       <c r="L271" s="9"/>
@@ -3662,9 +3664,9 @@
       <c r="A272" s="9"/>
       <c r="B272" s="9"/>
       <c r="C272" s="9"/>
+      <c r="E272" s="9"/>
+      <c r="F272" s="9"/>
       <c r="G272" s="9"/>
-      <c r="H272" s="9"/>
-      <c r="I272" s="9"/>
       <c r="J272" s="9"/>
       <c r="K272" s="9"/>
       <c r="L272" s="9"/>
@@ -3674,9 +3676,9 @@
       <c r="A273" s="9"/>
       <c r="B273" s="9"/>
       <c r="C273" s="9"/>
+      <c r="E273" s="9"/>
+      <c r="F273" s="9"/>
       <c r="G273" s="9"/>
-      <c r="H273" s="9"/>
-      <c r="I273" s="9"/>
       <c r="J273" s="9"/>
       <c r="K273" s="9"/>
       <c r="L273" s="9"/>
@@ -3686,9 +3688,9 @@
       <c r="A274" s="9"/>
       <c r="B274" s="9"/>
       <c r="C274" s="9"/>
+      <c r="E274" s="9"/>
+      <c r="F274" s="9"/>
       <c r="G274" s="9"/>
-      <c r="H274" s="9"/>
-      <c r="I274" s="9"/>
       <c r="J274" s="9"/>
       <c r="K274" s="9"/>
       <c r="L274" s="9"/>
@@ -3698,9 +3700,9 @@
       <c r="A275" s="9"/>
       <c r="B275" s="9"/>
       <c r="C275" s="9"/>
+      <c r="E275" s="9"/>
+      <c r="F275" s="9"/>
       <c r="G275" s="9"/>
-      <c r="H275" s="9"/>
-      <c r="I275" s="9"/>
       <c r="J275" s="9"/>
       <c r="K275" s="9"/>
       <c r="L275" s="9"/>
@@ -3710,9 +3712,9 @@
       <c r="A276" s="9"/>
       <c r="B276" s="9"/>
       <c r="C276" s="9"/>
+      <c r="E276" s="9"/>
+      <c r="F276" s="9"/>
       <c r="G276" s="9"/>
-      <c r="H276" s="9"/>
-      <c r="I276" s="9"/>
       <c r="J276" s="9"/>
       <c r="K276" s="9"/>
       <c r="L276" s="9"/>
@@ -3722,9 +3724,9 @@
       <c r="A277" s="9"/>
       <c r="B277" s="9"/>
       <c r="C277" s="9"/>
+      <c r="E277" s="9"/>
+      <c r="F277" s="9"/>
       <c r="G277" s="9"/>
-      <c r="H277" s="9"/>
-      <c r="I277" s="9"/>
       <c r="J277" s="9"/>
       <c r="K277" s="9"/>
       <c r="L277" s="9"/>
@@ -3734,9 +3736,9 @@
       <c r="A278" s="9"/>
       <c r="B278" s="9"/>
       <c r="C278" s="9"/>
+      <c r="E278" s="9"/>
+      <c r="F278" s="9"/>
       <c r="G278" s="9"/>
-      <c r="H278" s="9"/>
-      <c r="I278" s="9"/>
       <c r="J278" s="9"/>
       <c r="K278" s="9"/>
       <c r="L278" s="9"/>
@@ -3746,9 +3748,9 @@
       <c r="A279" s="9"/>
       <c r="B279" s="9"/>
       <c r="C279" s="9"/>
+      <c r="E279" s="9"/>
+      <c r="F279" s="9"/>
       <c r="G279" s="9"/>
-      <c r="H279" s="9"/>
-      <c r="I279" s="9"/>
       <c r="J279" s="9"/>
       <c r="K279" s="9"/>
       <c r="L279" s="9"/>
@@ -3758,9 +3760,9 @@
       <c r="A280" s="9"/>
       <c r="B280" s="9"/>
       <c r="C280" s="9"/>
+      <c r="E280" s="9"/>
+      <c r="F280" s="9"/>
       <c r="G280" s="9"/>
-      <c r="H280" s="9"/>
-      <c r="I280" s="9"/>
       <c r="J280" s="9"/>
       <c r="K280" s="9"/>
       <c r="L280" s="9"/>
@@ -3770,9 +3772,9 @@
       <c r="A281" s="9"/>
       <c r="B281" s="9"/>
       <c r="C281" s="9"/>
+      <c r="E281" s="9"/>
+      <c r="F281" s="9"/>
       <c r="G281" s="9"/>
-      <c r="H281" s="9"/>
-      <c r="I281" s="9"/>
       <c r="J281" s="9"/>
       <c r="K281" s="9"/>
       <c r="L281" s="9"/>
@@ -3782,9 +3784,9 @@
       <c r="A282" s="9"/>
       <c r="B282" s="9"/>
       <c r="C282" s="9"/>
+      <c r="E282" s="9"/>
+      <c r="F282" s="9"/>
       <c r="G282" s="9"/>
-      <c r="H282" s="9"/>
-      <c r="I282" s="9"/>
       <c r="J282" s="9"/>
       <c r="K282" s="9"/>
       <c r="L282" s="9"/>
@@ -3794,9 +3796,9 @@
       <c r="A283" s="9"/>
       <c r="B283" s="9"/>
       <c r="C283" s="9"/>
+      <c r="E283" s="9"/>
+      <c r="F283" s="9"/>
       <c r="G283" s="9"/>
-      <c r="H283" s="9"/>
-      <c r="I283" s="9"/>
       <c r="J283" s="9"/>
       <c r="K283" s="9"/>
       <c r="L283" s="9"/>
@@ -3806,9 +3808,9 @@
       <c r="A284" s="9"/>
       <c r="B284" s="9"/>
       <c r="C284" s="9"/>
+      <c r="E284" s="9"/>
+      <c r="F284" s="9"/>
       <c r="G284" s="9"/>
-      <c r="H284" s="9"/>
-      <c r="I284" s="9"/>
       <c r="J284" s="9"/>
       <c r="K284" s="9"/>
       <c r="L284" s="9"/>
@@ -3818,9 +3820,9 @@
       <c r="A285" s="9"/>
       <c r="B285" s="9"/>
       <c r="C285" s="9"/>
+      <c r="E285" s="9"/>
+      <c r="F285" s="9"/>
       <c r="G285" s="9"/>
-      <c r="H285" s="9"/>
-      <c r="I285" s="9"/>
       <c r="J285" s="9"/>
       <c r="K285" s="9"/>
       <c r="L285" s="9"/>
@@ -3830,9 +3832,9 @@
       <c r="A286" s="9"/>
       <c r="B286" s="9"/>
       <c r="C286" s="9"/>
+      <c r="E286" s="9"/>
+      <c r="F286" s="9"/>
       <c r="G286" s="9"/>
-      <c r="H286" s="9"/>
-      <c r="I286" s="9"/>
       <c r="J286" s="9"/>
       <c r="K286" s="9"/>
       <c r="L286" s="9"/>
@@ -4553,7 +4555,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>